<commit_message>
working on basic card layout
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -7,28 +7,80 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Deck" sheetId="1" r:id="rId1"/>
+    <sheet name="Opportunity" sheetId="1" r:id="rId1"/>
+    <sheet name="Alien" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Elf</t>
-  </si>
-  <si>
-    <t>Dwarf</t>
-  </si>
-  <si>
-    <t>ATK</t>
-  </si>
-  <si>
-    <t>DEF</t>
+    <t>Sieze Opportunity</t>
+  </si>
+  <si>
+    <t>Consume1</t>
+  </si>
+  <si>
+    <t>Consume2</t>
+  </si>
+  <si>
+    <t>Action1</t>
+  </si>
+  <si>
+    <t>Action2</t>
+  </si>
+  <si>
+    <t>Take an opportunity card from your pile and place it on your tableau.</t>
+  </si>
+  <si>
+    <t>Expand Options</t>
+  </si>
+  <si>
+    <t>Consume1Icon</t>
+  </si>
+  <si>
+    <t>Consume2Icon</t>
+  </si>
+  <si>
+    <t>electric</t>
+  </si>
+  <si>
+    <t>Deal +1 Opportunities</t>
+  </si>
+  <si>
+    <t>Required1</t>
+  </si>
+  <si>
+    <t>Required1Icon</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Buff</t>
+  </si>
+  <si>
+    <t>Required2</t>
+  </si>
+  <si>
+    <t>Required2Icon</t>
+  </si>
+  <si>
+    <t>glass-heart</t>
+  </si>
+  <si>
+    <t>Basic Factories</t>
+  </si>
+  <si>
+    <t>Action, Manufacturing</t>
   </si>
 </sst>
 </file>
@@ -72,9 +124,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,54 +437,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="14.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="63.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3">
         <v>3</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on more flexible cards
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,14 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Sieze Opportunity</t>
-  </si>
-  <si>
     <t>Consume1</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>electric</t>
   </si>
   <si>
-    <t>Deal +1 Opportunities</t>
-  </si>
-  <si>
     <t>Required1</t>
   </si>
   <si>
@@ -65,22 +59,43 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Buff</t>
-  </si>
-  <si>
     <t>Required2</t>
   </si>
   <si>
     <t>Required2Icon</t>
   </si>
   <si>
-    <t>glass-heart</t>
-  </si>
-  <si>
-    <t>Basic Factories</t>
-  </si>
-  <si>
     <t>Action, Manufacturing</t>
+  </si>
+  <si>
+    <t>Seize Opportunity</t>
+  </si>
+  <si>
+    <t>Auto Factory</t>
+  </si>
+  <si>
+    <t>Tech Factory</t>
+  </si>
+  <si>
+    <t>BuffType</t>
+  </si>
+  <si>
+    <t>Store1</t>
+  </si>
+  <si>
+    <t>Store1Icon</t>
+  </si>
+  <si>
+    <t>Store2</t>
+  </si>
+  <si>
+    <t>Store2Icon</t>
+  </si>
+  <si>
+    <t>While 5 Energy is stored, deal +1 Opportunities</t>
+  </si>
+  <si>
+    <t>city-car</t>
   </si>
 </sst>
 </file>
@@ -112,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -120,17 +135,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -437,108 +556,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="14.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="5">
+        <v>5</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="G5" s="3">
         <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got the card layouts mostly prototyped
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Action2</t>
   </si>
   <si>
-    <t>Take an opportunity card from your pile and place it on your tableau.</t>
-  </si>
-  <si>
     <t>Expand Options</t>
   </si>
   <si>
@@ -92,10 +89,73 @@
     <t>Store2Icon</t>
   </si>
   <si>
-    <t>While 5 Energy is stored, deal +1 Opportunities</t>
-  </si>
-  <si>
     <t>city-car</t>
+  </si>
+  <si>
+    <t>Action3</t>
+  </si>
+  <si>
+    <t>Tech School</t>
+  </si>
+  <si>
+    <t>Action, Organization</t>
+  </si>
+  <si>
+    <t>Hiring</t>
+  </si>
+  <si>
+    <t>miner</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>pencil-ruler</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Buff, Organization</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>tie</t>
+  </si>
+  <si>
+    <t>Decrease Energy cost by 1 per manager</t>
+  </si>
+  <si>
+    <t>Take an opportunity</t>
+  </si>
+  <si>
+    <t>While activated, 1 additional Opportunity card is available to you.</t>
+  </si>
+  <si>
+    <t>glass-heart</t>
+  </si>
+  <si>
+    <t>flying-beetle</t>
+  </si>
+  <si>
+    <t>grain-bundle</t>
+  </si>
+  <si>
+    <t>robot-golem</t>
+  </si>
+  <si>
+    <t>battle-tank</t>
+  </si>
+  <si>
+    <t>Something</t>
+  </si>
+  <si>
+    <t>Action, Awesome</t>
+  </si>
+  <si>
+    <t>Send a blight of flying beetles</t>
   </si>
 </sst>
 </file>
@@ -556,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,60 +633,61 @@
     <col min="7" max="7" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="18" max="18" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="M1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="O1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>3</v>
@@ -634,19 +695,22 @@
       <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="9">
         <v>3</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
@@ -660,58 +724,177 @@
       <c r="N2" s="11"/>
       <c r="O2" s="13"/>
       <c r="P2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="5">
         <v>5</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5">
         <v>2</v>
       </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="G5" s="3">
         <v>3</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="5">
+        <v>15</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bringing in ton of idea cards
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -134,28 +134,184 @@
     <t>While activated, 1 additional Opportunity card is available to you.</t>
   </si>
   <si>
-    <t>glass-heart</t>
-  </si>
-  <si>
-    <t>flying-beetle</t>
-  </si>
-  <si>
-    <t>grain-bundle</t>
-  </si>
-  <si>
-    <t>robot-golem</t>
-  </si>
-  <si>
-    <t>battle-tank</t>
-  </si>
-  <si>
-    <t>Something</t>
-  </si>
-  <si>
-    <t>Action, Awesome</t>
-  </si>
-  <si>
-    <t>Send a blight of flying beetles</t>
+    <t>Factory Automation</t>
+  </si>
+  <si>
+    <t>Buff, Manufacturing</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Increase Max factories to 3.</t>
+  </si>
+  <si>
+    <t>Exchange Opportunity</t>
+  </si>
+  <si>
+    <t>Swap one available Opportunity with another player from your purchase rows.</t>
+  </si>
+  <si>
+    <t>Efficient Operations</t>
+  </si>
+  <si>
+    <t>Middle Management</t>
+  </si>
+  <si>
+    <t>Maximum Managers is 2</t>
+  </si>
+  <si>
+    <t>Upper Management</t>
+  </si>
+  <si>
+    <t>Maximum Managers is 3</t>
+  </si>
+  <si>
+    <t>Executive Team</t>
+  </si>
+  <si>
+    <t>Maximum Managers is 4</t>
+  </si>
+  <si>
+    <t>Salvage Yards</t>
+  </si>
+  <si>
+    <t>Scrap a card on your tableau and place 3 energy on up to X different cards, where X is the number of workers.</t>
+  </si>
+  <si>
+    <t>Corporate Jet</t>
+  </si>
+  <si>
+    <t>Move this card and any cubes on it to another player.</t>
+  </si>
+  <si>
+    <t>Commercial Airline</t>
+  </si>
+  <si>
+    <t>Military Transport Network</t>
+  </si>
+  <si>
+    <t>Move up to 2 Soldiers per Officer from this card to a card on another player's tableau.</t>
+  </si>
+  <si>
+    <t>corporal</t>
+  </si>
+  <si>
+    <t>rank-3</t>
+  </si>
+  <si>
+    <t>Action, Military</t>
+  </si>
+  <si>
+    <t>Training Camp</t>
+  </si>
+  <si>
+    <t>Officer Academy</t>
+  </si>
+  <si>
+    <t>Buff, Military</t>
+  </si>
+  <si>
+    <t>Each craft in this fleet gains 1 extra Damage</t>
+  </si>
+  <si>
+    <t>Fleet Expansion</t>
+  </si>
+  <si>
+    <t>Fleet Admiral</t>
+  </si>
+  <si>
+    <t>Basic Fleet</t>
+  </si>
+  <si>
+    <t>interceptor-ship</t>
+  </si>
+  <si>
+    <t>spaceship</t>
+  </si>
+  <si>
+    <t>Fleet</t>
+  </si>
+  <si>
+    <t>Fleet, Military</t>
+  </si>
+  <si>
+    <t>Spread Efforts</t>
+  </si>
+  <si>
+    <t>Move this energy to up to 3 different cards on your tableau.</t>
+  </si>
+  <si>
+    <t>Social Media Campaign</t>
+  </si>
+  <si>
+    <t>Action, Internet</t>
+  </si>
+  <si>
+    <t>Media Disinformation</t>
+  </si>
+  <si>
+    <t>Decrease Panic by 1, then discard this card</t>
+  </si>
+  <si>
+    <t>This round, decrease Secrecy by 1 instead of by Panic, then discard this card after use.</t>
+  </si>
+  <si>
+    <t>Pass on Opportunity</t>
+  </si>
+  <si>
+    <t>Pass an available opportunity to the player on your left.</t>
+  </si>
+  <si>
+    <t>Pass an available opportunity to any player.</t>
+  </si>
+  <si>
+    <t>Action, Opportunity</t>
+  </si>
+  <si>
+    <t>Expedited Opportunity</t>
+  </si>
+  <si>
+    <t>Buff, Opportunity</t>
+  </si>
+  <si>
+    <t>Opportunity</t>
+  </si>
+  <si>
+    <t>When this action consumes energy, you may take an additional opportunity.</t>
+  </si>
+  <si>
+    <t>Search for New Opportunities</t>
+  </si>
+  <si>
+    <t>Action, Opportunity, Military</t>
+  </si>
+  <si>
+    <t>Discard an opportunity. Discard an additional opportunity per Officer.</t>
+  </si>
+  <si>
+    <t>New Strategic Directions</t>
+  </si>
+  <si>
+    <t>Discard an opportunity per Manager.</t>
+  </si>
+  <si>
+    <t>For each X Managers, X different players may discard one opportunity.</t>
+  </si>
+  <si>
+    <t>Shuffle your remaining opportunity cards.</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Action, Humanities</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>fountain-pen</t>
   </si>
 </sst>
 </file>
@@ -187,7 +343,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -268,49 +424,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,31 +820,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="18" max="18" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" style="19" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -650,52 +857,52 @@
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -704,7 +911,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="C2" s="9">
         <v>3</v>
@@ -712,189 +919,660 @@
       <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="8" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="J2" s="13"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="5">
+      <c r="G3" s="16">
         <v>5</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="H3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="16">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="D4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="16">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="D5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="18">
         <v>3</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="F5" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="16">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="D6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="20">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="K6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="16">
+        <v>3</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="5">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="16">
+        <v>2</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="18">
         <v>3</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="F7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="16">
+        <v>2</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="16">
+        <v>5</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="16">
+        <v>1</v>
+      </c>
+      <c r="O18" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="16">
+        <v>2</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="18">
+        <v>3</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="20">
+        <v>3</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="16">
+        <v>1</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="16">
+        <v>3</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="18">
+        <v>2</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="R21" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q22" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="16">
+        <v>2</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23" s="16">
+        <v>1</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16">
+        <v>3</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="16">
+        <v>5</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="16">
+        <v>2</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="16">
+        <v>2</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" s="20">
+        <v>3</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="P27" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q28" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="R28" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="16">
+        <v>1</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="20">
+        <v>2</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="16">
+        <v>2</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="16">
+        <v>1</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J30" s="20">
+        <v>4</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="P30" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="16">
+        <v>5</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="18">
+        <v>2</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="20">
+        <v>3</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L31" s="16">
+        <v>1</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="16">
+        <v>2</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="18">
+        <v>1</v>
+      </c>
+      <c r="F32" s="18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="J32" s="20">
         <v>2</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="K32" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" s="16">
         <v>3</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="M32" s="17" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="R8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="5">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="5">
-        <v>15</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="5">
-        <v>1</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TONs more cards. still brainstorming
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Salvage Yards</t>
   </si>
   <si>
-    <t>Scrap a card on your tableau and place 3 energy on up to X different cards, where X is the number of workers.</t>
-  </si>
-  <si>
     <t>Corporate Jet</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>Officer Academy</t>
   </si>
   <si>
-    <t>Buff, Military</t>
-  </si>
-  <si>
     <t>Each craft in this fleet gains 1 extra Damage</t>
   </si>
   <si>
@@ -254,9 +248,6 @@
     <t>Decrease Panic by 1, then discard this card</t>
   </si>
   <si>
-    <t>This round, decrease Secrecy by 1 instead of by Panic, then discard this card after use.</t>
-  </si>
-  <si>
     <t>Pass on Opportunity</t>
   </si>
   <si>
@@ -312,6 +303,129 @@
   </si>
   <si>
     <t>fountain-pen</t>
+  </si>
+  <si>
+    <t>Buff, Military, Fleet</t>
+  </si>
+  <si>
+    <t>Double the capacity of this Fleet.</t>
+  </si>
+  <si>
+    <t>Min 1</t>
+  </si>
+  <si>
+    <t>Min 0</t>
+  </si>
+  <si>
+    <t>This round, decrease Secrecy by 1 instead of by Panic, then discard this card.</t>
+  </si>
+  <si>
+    <t>Trash a card on your tableau, gain 3 energy on your Funding card, plus one per worker.</t>
+  </si>
+  <si>
+    <t>Decrease Energy costs by 1 per manager, down to a minimum of 2.</t>
+  </si>
+  <si>
+    <t>Interagency Collaborations</t>
+  </si>
+  <si>
+    <t>Buff, Military, Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Military OR Organization</t>
+  </si>
+  <si>
+    <t>Dangerous Mining</t>
+  </si>
+  <si>
+    <t>ore</t>
+  </si>
+  <si>
+    <t>Action, Minerals</t>
+  </si>
+  <si>
+    <t>Buff, Minerals</t>
+  </si>
+  <si>
+    <t>Improved Prospecting</t>
+  </si>
+  <si>
+    <t>Minerals</t>
+  </si>
+  <si>
+    <t>Produce +1 Minerals</t>
+  </si>
+  <si>
+    <t>Manual Prospecting</t>
+  </si>
+  <si>
+    <t>Produce 1 extra Minerals per worker, to a maximum of 3.</t>
+  </si>
+  <si>
+    <t>Mining Operations</t>
+  </si>
+  <si>
+    <t>Mining Company</t>
+  </si>
+  <si>
+    <t>Quest</t>
+  </si>
+  <si>
+    <t>Unknown Material Discovery</t>
+  </si>
+  <si>
+    <t>Converted Shipyard</t>
+  </si>
+  <si>
+    <t>Naval Shipyard</t>
+  </si>
+  <si>
+    <t>Action, Fleet, Organization</t>
+  </si>
+  <si>
+    <t>Action, Fleet, Military</t>
+  </si>
+  <si>
+    <t>Mining Logistics</t>
+  </si>
+  <si>
+    <t>3:1</t>
+  </si>
+  <si>
+    <t>2:3</t>
+  </si>
+  <si>
+    <t>2:1</t>
+  </si>
+  <si>
+    <t>There have been reports some unknown material uncovered somwhere. I don't know. Writer's block.</t>
+  </si>
+  <si>
+    <t>When this action produces Minerals, you may move those minerals to another action.</t>
+  </si>
+  <si>
+    <t>3:2</t>
+  </si>
+  <si>
+    <t>5:2</t>
+  </si>
+  <si>
+    <t>4:1</t>
+  </si>
+  <si>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>Mass Markets</t>
+  </si>
+  <si>
+    <t>5:30</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>5:20</t>
   </si>
 </sst>
 </file>
@@ -448,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -515,6 +629,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,11 +946,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,16 +963,16 @@
     <col min="6" max="6" width="16.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="29" style="19" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.42578125" style="19" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" style="19" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26" style="19" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
@@ -911,7 +1037,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" s="9">
         <v>3</v>
@@ -960,14 +1086,11 @@
       <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="16">
-        <v>3</v>
+      <c r="C4" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="18">
-        <v>1</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>24</v>
@@ -980,14 +1103,11 @@
       <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16">
-        <v>2</v>
+      <c r="C5" s="23" t="s">
+        <v>125</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" s="18">
-        <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>30</v>
@@ -1000,14 +1120,11 @@
       <c r="B6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="16">
-        <v>2</v>
+      <c r="C6" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" s="18">
-        <v>1</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>31</v>
@@ -1032,14 +1149,11 @@
       <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="16">
-        <v>2</v>
+      <c r="C7" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" s="18">
-        <v>3</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>29</v>
@@ -1064,8 +1178,8 @@
       <c r="B8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="16">
-        <v>1</v>
+      <c r="G8" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>35</v>
@@ -1147,15 +1261,27 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="G14" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>52</v>
       </c>
@@ -1168,25 +1294,19 @@
       <c r="D15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="16">
-        <v>1</v>
+      <c r="G15" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>29</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="N15" s="16">
-        <v>0</v>
-      </c>
-      <c r="O15" s="18" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>12</v>
@@ -1198,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M16" s="17" t="s">
         <v>35</v>
@@ -1206,7 +1326,7 @@
     </row>
     <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>12</v>
@@ -1218,7 +1338,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M17" s="17" t="s">
         <v>29</v>
@@ -1226,10 +1346,10 @@
     </row>
     <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
@@ -1238,36 +1358,33 @@
         <v>8</v>
       </c>
       <c r="I18" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="N18" s="16">
         <v>1</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="16">
-        <v>2</v>
+        <v>60</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>125</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="18">
-        <v>3</v>
-      </c>
       <c r="F19" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J19" s="20">
         <v>3</v>
@@ -1279,86 +1396,95 @@
         <v>1</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="16">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>129</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="18">
-        <v>2</v>
-      </c>
       <c r="F20" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="G21" s="16">
         <v>1</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="R21" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>64</v>
+        <v>96</v>
+      </c>
+      <c r="G22" s="16">
+        <v>2</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G23" s="16">
         <v>2</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N23" s="16">
         <v>1</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>12</v>
@@ -1370,15 +1496,15 @@
         <v>8</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="16">
         <v>5</v>
@@ -1387,15 +1513,15 @@
         <v>8</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" s="16">
         <v>2</v>
@@ -1404,15 +1530,15 @@
         <v>8</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="C27" s="16">
         <v>2</v>
@@ -1421,7 +1547,7 @@
         <v>8</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J27" s="20">
         <v>3</v>
@@ -1430,29 +1556,29 @@
         <v>8</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q28" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="R28" s="19" t="s">
         <v>84</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q28" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="R28" s="19" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C29" s="16">
         <v>1</v>
@@ -1460,14 +1586,14 @@
       <c r="D29" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="16">
-        <v>0</v>
+      <c r="G29" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J29" s="20">
         <v>2</v>
@@ -1476,15 +1602,15 @@
         <v>8</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C30" s="16">
         <v>2</v>
@@ -1492,14 +1618,14 @@
       <c r="D30" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="16">
-        <v>1</v>
+      <c r="G30" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>35</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J30" s="20">
         <v>4</v>
@@ -1508,27 +1634,24 @@
         <v>8</v>
       </c>
       <c r="P30" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="16">
-        <v>5</v>
+        <v>93</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>130</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="18">
-        <v>2</v>
-      </c>
       <c r="F31" s="18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J31" s="20">
         <v>3</v>
@@ -1540,7 +1663,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -1550,14 +1673,11 @@
       <c r="B32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="16">
-        <v>2</v>
+      <c r="C32" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>8</v>
-      </c>
-      <c r="E32" s="18">
-        <v>1</v>
       </c>
       <c r="F32" s="18" t="s">
         <v>31</v>
@@ -1573,6 +1693,265 @@
       </c>
       <c r="M32" s="17" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="J33" s="20">
+        <v>5</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L33" s="16">
+        <v>1</v>
+      </c>
+      <c r="M33" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="16">
+        <v>1</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q34" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="16">
+        <v>2</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="20">
+        <v>5</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="L35" s="16">
+        <v>3</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="16">
+        <v>3</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="R36" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q37" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="R37" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="16">
+        <v>1</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L39" s="16">
+        <v>1</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q40" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="R40" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="16">
+        <v>4</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="18">
+        <v>3</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J41" s="20">
+        <v>5</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="L41" s="16">
+        <v>1</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q42" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="R42" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
convert columns to resource names
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Consume2Icon</t>
   </si>
   <si>
-    <t>electric</t>
-  </si>
-  <si>
     <t>Required1</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Auto Factory</t>
   </si>
   <si>
-    <t>Tech Factory</t>
-  </si>
-  <si>
     <t>BuffType</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>Store2Icon</t>
   </si>
   <si>
-    <t>city-car</t>
-  </si>
-  <si>
     <t>Action3</t>
   </si>
   <si>
@@ -104,15 +95,6 @@
     <t>Hiring</t>
   </si>
   <si>
-    <t>miner</t>
-  </si>
-  <si>
-    <t>skills</t>
-  </si>
-  <si>
-    <t>pencil-ruler</t>
-  </si>
-  <si>
     <t>Management</t>
   </si>
   <si>
@@ -122,9 +104,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>tie</t>
-  </si>
-  <si>
     <t>Decrease Energy cost by 1 per manager</t>
   </si>
   <si>
@@ -191,12 +170,6 @@
     <t>Move up to 2 Soldiers per Officer from this card to a card on another player's tableau.</t>
   </si>
   <si>
-    <t>corporal</t>
-  </si>
-  <si>
-    <t>rank-3</t>
-  </si>
-  <si>
     <t>Action, Military</t>
   </si>
   <si>
@@ -218,12 +191,6 @@
     <t>Basic Fleet</t>
   </si>
   <si>
-    <t>interceptor-ship</t>
-  </si>
-  <si>
-    <t>spaceship</t>
-  </si>
-  <si>
     <t>Fleet</t>
   </si>
   <si>
@@ -299,12 +266,6 @@
     <t>Action, Humanities</t>
   </si>
   <si>
-    <t>read</t>
-  </si>
-  <si>
-    <t>fountain-pen</t>
-  </si>
-  <si>
     <t>Buff, Military, Fleet</t>
   </si>
   <si>
@@ -338,9 +299,6 @@
     <t>Dangerous Mining</t>
   </si>
   <si>
-    <t>ore</t>
-  </si>
-  <si>
     <t>Action, Minerals</t>
   </si>
   <si>
@@ -426,6 +384,42 @@
   </si>
   <si>
     <t>5:20</t>
+  </si>
+  <si>
+    <t>minerals</t>
+  </si>
+  <si>
+    <t>workers</t>
+  </si>
+  <si>
+    <t>cars</t>
+  </si>
+  <si>
+    <t>fighters</t>
+  </si>
+  <si>
+    <t>theologian</t>
+  </si>
+  <si>
+    <t>linguist</t>
+  </si>
+  <si>
+    <t>officer</t>
+  </si>
+  <si>
+    <t>engineers</t>
+  </si>
+  <si>
+    <t>officers</t>
+  </si>
+  <si>
+    <t>managers</t>
+  </si>
+  <si>
+    <t>soldiers</t>
+  </si>
+  <si>
+    <t>destroyers</t>
   </si>
 </sst>
 </file>
@@ -946,11 +940,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -990,16 +984,16 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>3</v>
@@ -1011,46 +1005,46 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C2" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>8</v>
+      <c r="D2" s="17" t="s">
+        <v>121</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
       <c r="I2" s="12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="10"/>
@@ -1067,891 +1061,886 @@
         <v>5</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="16">
         <v>5</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>125</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>30</v>
+        <v>130</v>
+      </c>
+      <c r="J5" s="20">
+        <v>5</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="L5" s="16">
+        <v>3</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="20">
-        <v>5</v>
+        <v>121</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="16">
+        <v>2</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="L6" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" s="16">
-        <v>2</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="16">
-        <v>1</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G11" s="16">
+        <v>5</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="16">
-        <v>5</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="16">
-        <v>1</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>121</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="R14" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="16">
         <v>1</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>101</v>
+        <v>47</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="16">
         <v>1</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C17" s="16">
         <v>1</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="N17" s="16">
+        <v>1</v>
+      </c>
+      <c r="O17" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="16">
+        <v>51</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J18" s="20">
+        <v>3</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="L18" s="16">
         <v>1</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>57</v>
-      </c>
       <c r="M18" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="N18" s="16">
-        <v>1</v>
-      </c>
-      <c r="O18" s="18" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>125</v>
+        <v>51</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="F19" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q20" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="20">
-        <v>3</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L19" s="16">
-        <v>1</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="R20" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G21" s="16">
-        <v>1</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>131</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="R21" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="R21" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>96</v>
+        <v>59</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="G22" s="16">
         <v>2</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q22" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="R22" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="N22" s="16">
+        <v>1</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="16">
+        <v>11</v>
+      </c>
+      <c r="C23" s="16">
+        <v>3</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="16">
+        <v>5</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="16">
         <v>2</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" s="16">
-        <v>1</v>
-      </c>
-      <c r="O23" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="16">
-        <v>3</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="16">
-        <v>5</v>
-      </c>
       <c r="D25" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C26" s="16">
         <v>2</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="J26" s="20">
+        <v>3</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="P26" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="R27" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="16">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="20">
+        <v>2</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="P28" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="C27" s="16">
-        <v>2</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="J27" s="20">
-        <v>3</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P27" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q28" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="R28" s="19" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C29" s="16">
+        <v>2</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" s="20">
+        <v>4</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="20">
+        <v>3</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="L30" s="16">
         <v>1</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J29" s="20">
-        <v>2</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="16">
-        <v>2</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="J30" s="20">
-        <v>4</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P30" s="19" t="s">
-        <v>90</v>
+      <c r="M30" s="17" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C31" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>94</v>
-      </c>
       <c r="J31" s="20">
+        <v>2</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="L31" s="16">
         <v>3</v>
       </c>
-      <c r="K31" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L31" s="16">
-        <v>1</v>
-      </c>
       <c r="M31" s="17" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="J32" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="L32" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="J33" s="20">
-        <v>5</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L33" s="16">
+        <v>91</v>
+      </c>
+      <c r="G33" s="16">
         <v>1</v>
       </c>
-      <c r="M33" s="17" t="s">
-        <v>107</v>
+      <c r="H33" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q33" s="21" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="G34" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q34" s="21" t="s">
-        <v>105</v>
+        <v>132</v>
+      </c>
+      <c r="J34" s="20">
+        <v>5</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="L34" s="16">
+        <v>3</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="G35" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" s="20">
-        <v>5</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="L35" s="16">
-        <v>3</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="Q35" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="R35" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" s="16">
-        <v>3</v>
+        <v>95</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="Q36" s="21" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q37" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="R37" s="19" t="s">
-        <v>114</v>
+        <v>94</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B38" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" s="16">
+        <v>1</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="L38" s="16">
+        <v>1</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q39" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="R39" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G39" s="16">
+      <c r="C40" s="16">
+        <v>4</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="18">
+        <v>3</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="J40" s="20">
+        <v>5</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="L40" s="16">
         <v>1</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J39" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" s="16">
-        <v>1</v>
-      </c>
-      <c r="M39" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q40" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="R40" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M40" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q41" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="R41" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="D42" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="J42" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="16">
-        <v>4</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="18">
-        <v>3</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="J41" s="20">
-        <v>5</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="L41" s="16">
-        <v>1</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q42" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="R42" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="J43" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="17" t="s">
-        <v>135</v>
+      <c r="K42" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unrolled a loop. Yes, more code. But readable?
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -35,18 +35,9 @@
     <t>Expand Options</t>
   </si>
   <si>
-    <t>Consume1Icon</t>
-  </si>
-  <si>
-    <t>Consume2Icon</t>
-  </si>
-  <si>
     <t>Required1</t>
   </si>
   <si>
-    <t>Required1Icon</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -56,9 +47,6 @@
     <t>Required2</t>
   </si>
   <si>
-    <t>Required2Icon</t>
-  </si>
-  <si>
     <t>Action, Manufacturing</t>
   </si>
   <si>
@@ -74,15 +62,9 @@
     <t>Store1</t>
   </si>
   <si>
-    <t>Store1Icon</t>
-  </si>
-  <si>
     <t>Store2</t>
   </si>
   <si>
-    <t>Store2Icon</t>
-  </si>
-  <si>
     <t>Action3</t>
   </si>
   <si>
@@ -420,6 +402,24 @@
   </si>
   <si>
     <t>destroyers</t>
+  </si>
+  <si>
+    <t>Consume1Resource</t>
+  </si>
+  <si>
+    <t>Store1Resource</t>
+  </si>
+  <si>
+    <t>Required1Resource</t>
+  </si>
+  <si>
+    <t>Consume2Resource</t>
+  </si>
+  <si>
+    <t>Store2Resource</t>
+  </si>
+  <si>
+    <t>Required2Resource</t>
   </si>
 </sst>
 </file>
@@ -943,8 +943,8 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,18 +952,18 @@
     <col min="1" max="1" width="28.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="19" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25.85546875" style="19" customWidth="1"/>
     <col min="17" max="17" width="24.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26" style="19" customWidth="1"/>
@@ -975,25 +975,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>3</v>
@@ -1002,49 +1002,49 @@
         <v>2</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C2" s="9">
         <v>3</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
       <c r="I2" s="12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="10"/>
@@ -1061,886 +1061,886 @@
         <v>5</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G3" s="16">
         <v>5</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J5" s="20">
         <v>5</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L5" s="16">
         <v>3</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J6" s="16">
         <v>2</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L6" s="16">
         <v>1</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G11" s="16">
         <v>5</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C12" s="16">
         <v>1</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" s="16">
         <v>1</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="16">
         <v>1</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" s="16">
         <v>1</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C17" s="16">
         <v>1</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="N17" s="16">
         <v>1</v>
       </c>
       <c r="O17" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J18" s="20">
         <v>3</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L18" s="16">
         <v>1</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G20" s="16">
         <v>1</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G21" s="16">
         <v>2</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G22" s="16">
         <v>2</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="N22" s="16">
         <v>1</v>
       </c>
       <c r="O22" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23" s="16">
         <v>3</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C24" s="16">
         <v>5</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C25" s="16">
         <v>2</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C26" s="16">
         <v>2</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J26" s="20">
         <v>3</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="Q27" s="21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="R27" s="19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C28" s="16">
         <v>1</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J28" s="20">
         <v>2</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="P28" s="19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C29" s="16">
         <v>2</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J29" s="20">
         <v>4</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J30" s="20">
         <v>3</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L30" s="16">
         <v>1</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J31" s="20">
         <v>2</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L31" s="16">
         <v>3</v>
       </c>
       <c r="M31" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J32" s="20">
         <v>5</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L32" s="16">
         <v>1</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G33" s="16">
         <v>1</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G34" s="16">
         <v>2</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J34" s="20">
         <v>5</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L34" s="16">
         <v>3</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G35" s="16">
         <v>3</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="Q35" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="R35" s="19" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="Q36" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C37" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G38" s="16">
         <v>1</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J38" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="K38" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>124</v>
       </c>
       <c r="L38" s="16">
         <v>1</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Q39" s="21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="R39" s="19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C40" s="16">
         <v>4</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E40" s="18">
         <v>3</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J40" s="20">
         <v>5</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L40" s="16">
         <v>1</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Q41" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="R41" s="19" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="K42" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>125</v>
-      </c>
       <c r="M42" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more conversions to new formats
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -420,6 +420,18 @@
   </si>
   <si>
     <t>Required2Resource</t>
+  </si>
+  <si>
+    <t>4:3</t>
+  </si>
+  <si>
+    <t>5:1</t>
+  </si>
+  <si>
+    <t>5:3</t>
+  </si>
+  <si>
+    <t>Max 3</t>
   </si>
 </sst>
 </file>
@@ -943,8 +955,8 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1098,9 @@
       <c r="D4" s="17" t="s">
         <v>115</v>
       </c>
+      <c r="E4" s="18" t="s">
+        <v>138</v>
+      </c>
       <c r="F4" s="18" t="s">
         <v>119</v>
       </c>
@@ -1106,14 +1121,11 @@
       <c r="F5" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="J5" s="20">
-        <v>5</v>
+      <c r="J5" s="26" t="s">
+        <v>137</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="L5" s="16">
-        <v>3</v>
       </c>
       <c r="M5" s="17" t="s">
         <v>124</v>
@@ -1135,14 +1147,11 @@
       <c r="F6" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="J6" s="16">
-        <v>2</v>
+      <c r="J6" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="L6" s="16">
-        <v>1</v>
       </c>
       <c r="M6" s="17" t="s">
         <v>126</v>
@@ -1372,14 +1381,11 @@
       <c r="F18" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="J18" s="20">
-        <v>3</v>
+      <c r="J18" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="L18" s="16">
-        <v>1</v>
       </c>
       <c r="M18" s="17" t="s">
         <v>125</v>
@@ -1642,14 +1648,11 @@
       <c r="F30" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="J30" s="20">
-        <v>3</v>
+      <c r="J30" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="L30" s="16">
-        <v>1</v>
       </c>
       <c r="M30" s="17" t="s">
         <v>121</v>
@@ -1671,14 +1674,11 @@
       <c r="F31" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J31" s="20">
-        <v>2</v>
+      <c r="J31" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="K31" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="L31" s="16">
-        <v>3</v>
       </c>
       <c r="M31" s="17" t="s">
         <v>118</v>
@@ -1700,14 +1700,11 @@
       <c r="F32" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J32" s="20">
-        <v>5</v>
+      <c r="J32" s="26" t="s">
+        <v>136</v>
       </c>
       <c r="K32" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="L32" s="16">
-        <v>1</v>
       </c>
       <c r="M32" s="17" t="s">
         <v>117</v>
@@ -1752,14 +1749,11 @@
       <c r="H34" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="J34" s="20">
-        <v>5</v>
+      <c r="J34" s="25" t="s">
+        <v>137</v>
       </c>
       <c r="K34" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="L34" s="16">
-        <v>3</v>
       </c>
       <c r="M34" s="17" t="s">
         <v>120</v>
@@ -1850,9 +1844,6 @@
       <c r="K38" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="L38" s="16">
-        <v>1</v>
-      </c>
       <c r="M38" s="17" t="s">
         <v>126</v>
       </c>
@@ -1878,26 +1869,20 @@
       <c r="B40" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="16">
-        <v>4</v>
+      <c r="C40" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="18">
-        <v>3</v>
-      </c>
       <c r="F40" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="J40" s="20">
-        <v>5</v>
+      <c r="J40" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="K40" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="L40" s="16">
-        <v>1</v>
       </c>
       <c r="M40" s="17" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
minor tweaks, add some maxes
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -386,9 +386,6 @@
     <t>linguist</t>
   </si>
   <si>
-    <t>officer</t>
-  </si>
-  <si>
     <t>engineers</t>
   </si>
   <si>
@@ -432,6 +429,15 @@
   </si>
   <si>
     <t>Max 3</t>
+  </si>
+  <si>
+    <t>Max 2</t>
+  </si>
+  <si>
+    <t>Max 5</t>
+  </si>
+  <si>
+    <t>Max 4</t>
   </si>
 </sst>
 </file>
@@ -955,8 +961,8 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,19 +999,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>3</v>
@@ -1014,19 +1020,19 @@
         <v>2</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>4</v>
@@ -1099,7 +1105,7 @@
         <v>115</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>119</v>
@@ -1119,16 +1125,16 @@
         <v>115</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>115</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1154,7 +1160,7 @@
         <v>115</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1168,7 +1174,7 @@
         <v>79</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="21" t="s">
         <v>22</v>
@@ -1267,7 +1273,7 @@
         <v>79</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q13" s="21" t="s">
         <v>22</v>
@@ -1316,7 +1322,7 @@
         <v>41</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1356,13 +1362,13 @@
         <v>44</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N17" s="16">
         <v>1</v>
       </c>
       <c r="O17" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1379,7 +1385,7 @@
         <v>115</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J18" s="26" t="s">
         <v>104</v>
@@ -1388,7 +1394,7 @@
         <v>115</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1405,7 +1411,7 @@
         <v>115</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1419,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q20" s="21" t="s">
         <v>52</v>
@@ -1439,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q21" s="21" t="s">
         <v>52</v>
@@ -1455,6 +1461,9 @@
       <c r="B22" s="15" t="s">
         <v>53</v>
       </c>
+      <c r="E22" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="F22" s="18" t="s">
         <v>120</v>
       </c>
@@ -1462,16 +1471,19 @@
         <v>2</v>
       </c>
       <c r="H22" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="M22" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>128</v>
       </c>
       <c r="N22" s="16">
         <v>1</v>
       </c>
       <c r="O22" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1558,9 +1570,6 @@
       <c r="B27" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>115</v>
-      </c>
       <c r="Q27" s="21" t="s">
         <v>66</v>
       </c>
@@ -1585,7 +1594,7 @@
         <v>80</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I28" s="19" t="s">
         <v>70</v>
@@ -1617,7 +1626,7 @@
         <v>79</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>72</v>
@@ -1672,7 +1681,7 @@
         <v>115</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J31" s="26" t="s">
         <v>105</v>
@@ -1697,14 +1706,20 @@
       <c r="D32" s="17" t="s">
         <v>118</v>
       </c>
+      <c r="E32" s="18" t="s">
+        <v>139</v>
+      </c>
       <c r="F32" s="18" t="s">
         <v>117</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K32" s="17" t="s">
         <v>115</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="M32" s="17" t="s">
         <v>117</v>
@@ -1721,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q33" s="21" t="s">
         <v>86</v>
@@ -1740,6 +1755,9 @@
       <c r="D34" s="17" t="s">
         <v>117</v>
       </c>
+      <c r="E34" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="F34" s="18" t="s">
         <v>120</v>
       </c>
@@ -1747,13 +1765,16 @@
         <v>2</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K34" s="17" t="s">
         <v>117</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="M34" s="17" t="s">
         <v>120</v>
@@ -1836,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>112</v>
@@ -1845,7 +1866,7 @@
         <v>118</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -1870,22 +1891,28 @@
         <v>102</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>117</v>
       </c>
+      <c r="E40" s="18" t="s">
+        <v>140</v>
+      </c>
       <c r="F40" s="18" t="s">
         <v>120</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K40" s="17" t="s">
         <v>117</v>
       </c>
+      <c r="L40" s="16" t="s">
+        <v>137</v>
+      </c>
       <c r="M40" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
better formatting of buff types
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -964,12 +964,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1055,7 +1054,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1084,7 @@
       <c r="Q2" s="12"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>12</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>39</v>
       </c>
@@ -1316,7 +1315,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>40</v>
       </c>
@@ -1336,7 +1335,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>42</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>46</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>47</v>
       </c>
@@ -1465,7 +1464,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>51</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>54</v>
       </c>
@@ -1514,7 +1513,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>56</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>58</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>60</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>71</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>68</v>
       </c>
@@ -1652,7 +1651,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
         <v>75</v>
       </c>
@@ -1678,7 +1677,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>17</v>
       </c>
@@ -1704,7 +1703,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>87</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
         <v>99</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
         <v>95</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
         <v>96</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
         <v>98</v>
       </c>
@@ -1890,11 +1889,8 @@
       <c r="Q39" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="R39" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>100</v>
       </c>
@@ -1940,7 +1936,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
         <v>113</v>
       </c>
@@ -1967,18 +1963,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S42">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Buff, Manufacturing"/>
-        <filter val="Buff, Military, Fleet"/>
-        <filter val="Buff, Military, Organization"/>
-        <filter val="Buff, Minerals"/>
-        <filter val="Buff, Opportunity"/>
-        <filter val="Buff, Organization"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S42"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new ideas! motivation mat and friends
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2348C18C-50EB-4D4A-8209-0C50A781B44E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1E2578-D777-46CC-9A39-331AFB17DEED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opportunity" sheetId="1" r:id="rId1"/>
     <sheet name="Alien" sheetId="2" r:id="rId2"/>
-    <sheet name="Panic" sheetId="3" r:id="rId3"/>
-    <sheet name="Secrecy" sheetId="5" r:id="rId4"/>
-    <sheet name="Quests" sheetId="4" r:id="rId5"/>
+    <sheet name="Hurts" sheetId="6" r:id="rId3"/>
+    <sheet name="Panic" sheetId="3" r:id="rId4"/>
+    <sheet name="Secrecy" sheetId="5" r:id="rId5"/>
+    <sheet name="Quests" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Opportunity!$A$1:$S$47</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="297">
   <si>
     <t>Name</t>
   </si>
@@ -567,9 +568,6 @@
     <t>Managers and officers on this card are equivalent.</t>
   </si>
   <si>
-    <t>When this action produces Minerals, you may move up to 3 minerals to another action.</t>
-  </si>
-  <si>
     <t>Global Mining Efficiencies</t>
   </si>
   <si>
@@ -627,9 +625,6 @@
     <t>Recon Shuttle</t>
   </si>
   <si>
-    <t>explore</t>
-  </si>
-  <si>
     <t>Action, Military, Recon</t>
   </si>
   <si>
@@ -646,6 +641,279 @@
   </si>
   <si>
     <t>interpretation</t>
+  </si>
+  <si>
+    <t>When this action produces Minerals, you may move up to 3 minerals to another action for free</t>
+  </si>
+  <si>
+    <t>Stock Markets</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Strange Vibrations</t>
+  </si>
+  <si>
+    <t>recons</t>
+  </si>
+  <si>
+    <t>Theology</t>
+  </si>
+  <si>
+    <t>Military</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Farming</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Cosmic Fertilizer</t>
+  </si>
+  <si>
+    <t>Remote Mountains</t>
+  </si>
+  <si>
+    <t>Famous Mountains</t>
+  </si>
+  <si>
+    <t>Crusade</t>
+  </si>
+  <si>
+    <t>Slave Labor</t>
+  </si>
+  <si>
+    <t>The Shrine</t>
+  </si>
+  <si>
+    <t>Hallucinogenic Drugs</t>
+  </si>
+  <si>
+    <t>Origins of the Universe</t>
+  </si>
+  <si>
+    <t>Proselytizing Nanites</t>
+  </si>
+  <si>
+    <t>Gravity Wells</t>
+  </si>
+  <si>
+    <t>Death Ray</t>
+  </si>
+  <si>
+    <t>Secret of the Ancients</t>
+  </si>
+  <si>
+    <t>Staging Area</t>
+  </si>
+  <si>
+    <t>Plague</t>
+  </si>
+  <si>
+    <t>Nuclear Mining</t>
+  </si>
+  <si>
+    <t>Megastructures</t>
+  </si>
+  <si>
+    <t>It's Made of People</t>
+  </si>
+  <si>
+    <t>Genetic Engineering</t>
+  </si>
+  <si>
+    <t>Earthen Sculpture</t>
+  </si>
+  <si>
+    <t>Reapers</t>
+  </si>
+  <si>
+    <t>Biofuel</t>
+  </si>
+  <si>
+    <t>Terraforming Earth</t>
+  </si>
+  <si>
+    <t>Utopian Society</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Assassination</t>
+  </si>
+  <si>
+    <t>Kill an important person</t>
+  </si>
+  <si>
+    <t>Destroy Mountain</t>
+  </si>
+  <si>
+    <t>Lower Energy Debuff</t>
+  </si>
+  <si>
+    <t>Sabotage</t>
+  </si>
+  <si>
+    <t>Destroy some crafts</t>
+  </si>
+  <si>
+    <t>Endgame Name</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Reason1</t>
+  </si>
+  <si>
+    <t>Reason2</t>
+  </si>
+  <si>
+    <t>d20</t>
+  </si>
+  <si>
+    <t>d12</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>Red: -1</t>
+  </si>
+  <si>
+    <t>Red: -1, Purple: -1</t>
+  </si>
+  <si>
+    <t>Red: -2, Purple: -1</t>
+  </si>
+  <si>
+    <t>Red: -2, Purple: -2</t>
+  </si>
+  <si>
+    <t>Attack Name</t>
+  </si>
+  <si>
+    <t>Purple: -1</t>
+  </si>
+  <si>
+    <t>Purple: -2, Green: -1</t>
+  </si>
+  <si>
+    <t>Purple: -3, Green: -2</t>
+  </si>
+  <si>
+    <t>Purple: -3, Green: -3</t>
+  </si>
+  <si>
+    <t>Green: -1</t>
+  </si>
+  <si>
+    <t>Black: -1</t>
+  </si>
+  <si>
+    <t>Yellow: -1</t>
+  </si>
+  <si>
+    <t>Blue: -1</t>
+  </si>
+  <si>
+    <t>Purple: -1, Blue: -1</t>
+  </si>
+  <si>
+    <t>Purple: -1, Blue: -2</t>
+  </si>
+  <si>
+    <t>Purple: -1, , Blue: -2</t>
+  </si>
+  <si>
+    <t>Red: -1, Blue: -2</t>
+  </si>
+  <si>
+    <t>Green: -1, Blue: -1</t>
+  </si>
+  <si>
+    <t>Green: -2, , Blue: -1</t>
+  </si>
+  <si>
+    <t>Green: -1, , Blue: -2</t>
+  </si>
+  <si>
+    <t>Black: -1, Blue: -2</t>
+  </si>
+  <si>
+    <t>Black: -2, Blue: -1</t>
+  </si>
+  <si>
+    <t>Black: -2, Blue: -2</t>
+  </si>
+  <si>
+    <t>Purple: -1, Yellow: -1</t>
+  </si>
+  <si>
+    <t>Purple: -2, , Yellow: -1</t>
+  </si>
+  <si>
+    <t>Purple: -2, Yellow: -3</t>
+  </si>
+  <si>
+    <t>Red: -1, Yellow: -1</t>
+  </si>
+  <si>
+    <t>Green: -1, Yellow: -2</t>
+  </si>
+  <si>
+    <t>Green: -1, Yellow: -3</t>
+  </si>
+  <si>
+    <t>Black: -1, Yellow: -1</t>
+  </si>
+  <si>
+    <t>Blue: -1, Yellow: -1</t>
+  </si>
+  <si>
+    <t>Purple: -1, Black: -1</t>
+  </si>
+  <si>
+    <t>Red: -1, Black: -1</t>
+  </si>
+  <si>
+    <t>Red: -1, Black: -2</t>
+  </si>
+  <si>
+    <t>Red: -2, Black: -2</t>
+  </si>
+  <si>
+    <t>Puzzling Miracles</t>
+  </si>
+  <si>
+    <t>Hailing Fireballs</t>
+  </si>
+  <si>
+    <t>Scattered Poisonings</t>
+  </si>
+  <si>
+    <t>Dimensional Portals</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>Fear the Other</t>
+  </si>
+  <si>
+    <t>Zombie Analysts</t>
   </si>
 </sst>
 </file>
@@ -782,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -870,6 +1138,11 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1209,11 +1482,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S67"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,7 +1633,7 @@
     </row>
     <row r="4" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -1389,7 +1662,7 @@
       <c r="N4" s="14"/>
       <c r="O4" s="16"/>
       <c r="P4" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q4" s="13"/>
       <c r="R4" s="18"/>
@@ -1413,7 +1686,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
       <c r="I5" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J5" s="17"/>
       <c r="K5" s="15"/>
@@ -1545,7 +1818,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>142</v>
@@ -1646,245 +1919,244 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="29" t="str">
+        <v>202</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="24" t="str">
         <f>"3:1"</f>
         <v>3:1</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="G13" s="14">
-        <v>2</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="N13" s="14">
-        <v>1</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="P13" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>110</v>
-      </c>
       <c r="D14" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>103</v>
+        <v>210</v>
+      </c>
+      <c r="P14" s="13" t="str">
+        <f>"-1 Secrecy"</f>
+        <v>-1 Secrecy</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>86</v>
+        <v>178</v>
+      </c>
+      <c r="C15" s="29" t="str">
+        <f>"3:1"</f>
+        <v>3:1</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
       <c r="G15" s="14">
         <v>2</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>97</v>
+        <v>172</v>
+      </c>
+      <c r="N15" s="14">
+        <v>1</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>84</v>
+        <v>97</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="M16" s="15" t="s">
-        <v>172</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="24">
-        <v>5</v>
+        <v>82</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="27"/>
-      <c r="I17" s="13" t="s">
-        <v>68</v>
+        <v>94</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="14">
+        <v>2</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="24">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="13" t="s">
-        <v>51</v>
+      <c r="F18" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="29" t="str">
+      <c r="C19" s="24">
+        <v>5</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="I19" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="24">
+        <v>2</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="29" t="str">
         <f>"5:6"</f>
         <v>5:6</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="J19" s="17" t="str">
+      <c r="J21" s="17" t="str">
         <f>"3:4"</f>
         <v>3:4</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K21" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M21" s="15" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="24">
-        <v>2</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="24">
-        <v>1</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>35</v>
+        <v>183</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="C22" s="24">
         <v>2</v>
@@ -1892,71 +2164,77 @@
       <c r="D22" s="15" t="s">
         <v>92</v>
       </c>
+      <c r="H22" s="15" t="s">
+        <v>172</v>
+      </c>
       <c r="I22" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>119</v>
       </c>
       <c r="C23" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F23" s="15"/>
+      <c r="G23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>95</v>
+      </c>
       <c r="I23" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="E24" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="J24" s="20"/>
+        <v>119</v>
+      </c>
+      <c r="C24" s="24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="E25" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>97</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C25" s="24">
+        <v>3</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="27"/>
       <c r="H25" s="27"/>
-      <c r="J25" s="20"/>
-      <c r="L25" s="14" t="s">
-        <v>120</v>
+      <c r="I25" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="M25" s="15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
@@ -1997,7 +2275,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>96</v>
@@ -2114,122 +2392,122 @@
         <v>92</v>
       </c>
       <c r="P31" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C32" s="24" t="str">
+        <f>"2:1"</f>
+        <v>2:1</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="P32" s="13" t="str">
+        <f>"-1 Secrecy for each Military Problem discovered"</f>
+        <v>-1 Secrecy for each Military Problem discovered</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="24" t="str">
+        <f>"5:1"</f>
+        <v>5:1</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="O33" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B34" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="24" t="str">
+      <c r="C34" s="24" t="str">
         <f>"3:1"</f>
         <v>3:1</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="16" t="s">
+      <c r="D34" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G34" s="14">
         <v>2</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H34" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="N32" s="14">
+      <c r="N34" s="14">
         <v>1</v>
       </c>
-      <c r="O32" s="16" t="s">
+      <c r="O34" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="P32" s="13" t="s">
+      <c r="P34" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="19" t="str">
+      <c r="C35" s="19" t="str">
         <f>"1:2"</f>
         <v>1:2</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D35" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F35" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="J35" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="K33" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="L33" s="14" t="s">
+      <c r="K35" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L35" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="M33" s="15" t="s">
+      <c r="M35" s="15" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A34" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="G35" s="14">
-        <v>1</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="M35" s="15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
@@ -2239,162 +2517,177 @@
       <c r="B36" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="24" t="str">
+      <c r="C36" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="14">
+        <v>1</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="24" t="str">
         <f>"6:3"</f>
         <v>6:3</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="16" t="s">
+      <c r="D38" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G38" s="14">
         <v>2</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H38" s="15" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="J37" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="M37" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A38" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="J38" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="K38" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="M38" s="15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="24">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="14">
-        <v>2</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="N39" s="14">
-        <v>1</v>
-      </c>
-      <c r="O39" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="P39" s="13" t="s">
-        <v>163</v>
+        <v>92</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="R40" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="S40" s="13" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C41" s="24">
+        <v>3</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="14">
+        <v>2</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="N41" s="14">
         <v>1</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="R41" s="18" t="s">
-        <v>166</v>
+      <c r="O41" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P41" s="13" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F42" s="15"/>
       <c r="R42" s="18" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
       <c r="S42" s="13" t="s">
-        <v>195</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
       <c r="C43" s="24">
         <v>1</v>
@@ -2404,169 +2697,178 @@
       </c>
       <c r="F43" s="15"/>
       <c r="I43" s="13" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="R43" s="18" t="s">
-        <v>26</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" s="14">
-        <v>1</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>100</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="F44" s="27"/>
       <c r="R44" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="S44" s="28" t="s">
-        <v>187</v>
+        <v>126</v>
+      </c>
+      <c r="S44" s="13" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="14">
-        <v>2</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="C45" s="24">
+        <v>1</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="27"/>
+      <c r="I45" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="R45" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="S45" s="13" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="G46" s="14">
+        <v>1</v>
       </c>
       <c r="H46" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="O46" s="16" t="s">
-        <v>101</v>
-      </c>
       <c r="R46" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="S46" s="13" t="s">
-        <v>180</v>
+        <v>45</v>
+      </c>
+      <c r="S46" s="28" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>174</v>
+        <v>42</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F47" s="15"/>
+      <c r="G47" s="14">
+        <v>2</v>
+      </c>
       <c r="H47" s="15" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="R47" s="18" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="S47" s="13" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>122</v>
+        <v>71</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="O48" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="R48" s="18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S48" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G49" s="14">
-        <v>1</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F49" s="27"/>
       <c r="H49" s="15" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="R49" s="18" t="s">
+        <v>76</v>
       </c>
       <c r="S49" s="13" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="R50" s="18" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="S50" s="13" t="s">
-        <v>23</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
-        <v>28</v>
+        <v>181</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="R51" s="18" t="s">
-        <v>22</v>
+        <v>122</v>
+      </c>
+      <c r="G51" s="14">
+        <v>1</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="S51" s="13" t="s">
-        <v>29</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="H52" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="R52" s="18" t="s">
         <v>22</v>
       </c>
       <c r="S52" s="13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>21</v>
@@ -2575,80 +2877,72 @@
         <v>22</v>
       </c>
       <c r="S53" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R54" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="S54" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A55" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="R55" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="S55" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A56" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B56" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E56" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F54" s="16" t="s">
+      <c r="F56" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="14">
+      <c r="G56" s="14">
         <v>2</v>
       </c>
-      <c r="H54" s="15" t="s">
+      <c r="H56" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="L54" s="14" t="s">
+      <c r="L56" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="M54" s="15" t="s">
+      <c r="M56" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="N54" s="14">
+      <c r="N56" s="14">
         <v>1</v>
       </c>
-      <c r="O54" s="16" t="s">
+      <c r="O56" s="16" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A55" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="O55" s="27"/>
-      <c r="P55" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q55" s="26"/>
-      <c r="S55" s="26"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A56" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="O56" s="27"/>
-      <c r="P56" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q56" s="26"/>
-      <c r="S56" s="26"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B57" s="26" t="s">
         <v>127</v>
@@ -2659,14 +2953,14 @@
       </c>
       <c r="O57" s="27"/>
       <c r="P57" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q57" s="26"/>
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B58" s="26" t="s">
         <v>127</v>
@@ -2677,14 +2971,14 @@
       </c>
       <c r="O58" s="27"/>
       <c r="P58" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q58" s="26"/>
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="26" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B59" s="26" t="s">
         <v>127</v>
@@ -2695,149 +2989,170 @@
       </c>
       <c r="O59" s="27"/>
       <c r="P59" s="26" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="Q59" s="26"/>
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A60" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="24">
-        <v>1</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G60" s="14">
-        <v>1</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="I60" s="13" t="s">
-        <v>152</v>
-      </c>
+      <c r="A60" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="O60" s="27"/>
+      <c r="P60" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q60" s="26"/>
+      <c r="S60" s="26"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A61" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="O61" s="27"/>
+      <c r="P61" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q61" s="26"/>
+      <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C62" s="24">
-        <v>1</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H62" s="15" t="s">
-        <v>173</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C62" s="25"/>
+      <c r="E62" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J62" s="20"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
-        <v>205</v>
+        <v>124</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C63" s="24" t="str">
-        <f>"2:1"</f>
-        <v>2:1</v>
+        <v>126</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="E63" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="P63" s="13" t="str">
-        <f>"-1 Secrecy for each Military Problem discovered"</f>
-        <v>-1 Secrecy for each Military Problem discovered</v>
+        <v>97</v>
+      </c>
+      <c r="J63" s="20"/>
+      <c r="L63" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="M63" s="15" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
-        <v>203</v>
+        <v>150</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C64" s="24" t="str">
-        <f>"3:1"</f>
-        <v>3:1</v>
+        <v>151</v>
+      </c>
+      <c r="C64" s="24">
+        <v>1</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F64" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="P64" s="13" t="str">
-        <f>"-1 Secrecy"</f>
-        <v>-1 Secrecy</v>
+      <c r="G64" s="14">
+        <v>1</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
-        <v>200</v>
+        <v>79</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C65" s="24" t="str">
-        <f>"5:1"</f>
-        <v>5:1</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="N65" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="O65" s="16" t="s">
-        <v>97</v>
+        <v>78</v>
+      </c>
+      <c r="F65" s="27"/>
+      <c r="Q65" s="13" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R66" s="18" t="s">
         <v>78</v>
       </c>
       <c r="S66" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
-        <v>79</v>
+        <v>207</v>
       </c>
       <c r="B67" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A68" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B68" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F67" s="27"/>
-      <c r="Q67" s="13" t="s">
-        <v>196</v>
+      <c r="G68" s="14">
+        <v>3</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A69" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A70" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2846,8 +3161,8 @@
       <sortCondition ref="B2:B47"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S67">
-    <sortCondition ref="B2:B67"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S66">
+    <sortCondition ref="B2:B66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2856,17 +3171,613 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="G2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F4" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" t="s">
+        <v>268</v>
+      </c>
+      <c r="H4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" t="s">
+        <v>278</v>
+      </c>
+      <c r="H5" t="s">
+        <v>279</v>
+      </c>
+      <c r="I5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" t="s">
+        <v>286</v>
+      </c>
+      <c r="H6" t="s">
+        <v>286</v>
+      </c>
+      <c r="I6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" t="s">
+        <v>296</v>
+      </c>
+      <c r="F7" t="s">
+        <v>260</v>
+      </c>
+      <c r="G7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" t="s">
+        <v>255</v>
+      </c>
+      <c r="G8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" t="s">
+        <v>255</v>
+      </c>
+      <c r="G9" t="s">
+        <v>287</v>
+      </c>
+      <c r="H9" t="s">
+        <v>288</v>
+      </c>
+      <c r="I9" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" t="s">
+        <v>255</v>
+      </c>
+      <c r="G10" t="s">
+        <v>271</v>
+      </c>
+      <c r="H10" t="s">
+        <v>271</v>
+      </c>
+      <c r="I10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H11" t="s">
+        <v>281</v>
+      </c>
+      <c r="I11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" t="s">
+        <v>255</v>
+      </c>
+      <c r="G12" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" t="s">
+        <v>255</v>
+      </c>
+      <c r="I12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F13" t="s">
+        <v>264</v>
+      </c>
+      <c r="G13" t="s">
+        <v>264</v>
+      </c>
+      <c r="H13" t="s">
+        <v>264</v>
+      </c>
+      <c r="I13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" t="s">
+        <v>232</v>
+      </c>
+      <c r="F14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G14" t="s">
+        <v>272</v>
+      </c>
+      <c r="H14" t="s">
+        <v>273</v>
+      </c>
+      <c r="I14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" t="s">
+        <v>282</v>
+      </c>
+      <c r="H15" t="s">
+        <v>283</v>
+      </c>
+      <c r="I15" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16" t="s">
+        <v>234</v>
+      </c>
+      <c r="F16" t="s">
+        <v>264</v>
+      </c>
+      <c r="G16" t="s">
+        <v>264</v>
+      </c>
+      <c r="H16" t="s">
+        <v>264</v>
+      </c>
+      <c r="I16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F17" t="s">
+        <v>265</v>
+      </c>
+      <c r="G17" t="s">
+        <v>275</v>
+      </c>
+      <c r="H17" t="s">
+        <v>276</v>
+      </c>
+      <c r="I17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" t="s">
+        <v>236</v>
+      </c>
+      <c r="F18" t="s">
+        <v>265</v>
+      </c>
+      <c r="G18" t="s">
+        <v>284</v>
+      </c>
+      <c r="H18" t="s">
+        <v>284</v>
+      </c>
+      <c r="I18" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19" t="s">
+        <v>237</v>
+      </c>
+      <c r="F19" t="s">
+        <v>265</v>
+      </c>
+      <c r="G19" t="s">
+        <v>265</v>
+      </c>
+      <c r="H19" t="s">
+        <v>265</v>
+      </c>
+      <c r="I19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F20" t="s">
+        <v>267</v>
+      </c>
+      <c r="G20" t="s">
+        <v>285</v>
+      </c>
+      <c r="H20" t="s">
+        <v>285</v>
+      </c>
+      <c r="I20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C21" t="s">
+        <v>239</v>
+      </c>
+      <c r="F21" t="s">
+        <v>267</v>
+      </c>
+      <c r="G21" t="s">
+        <v>267</v>
+      </c>
+      <c r="H21" t="s">
+        <v>267</v>
+      </c>
+      <c r="I21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" t="s">
+        <v>294</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" t="s">
+        <v>266</v>
+      </c>
+      <c r="G22" t="s">
+        <v>266</v>
+      </c>
+      <c r="H22" t="s">
+        <v>266</v>
+      </c>
+      <c r="I22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7524C21F-D212-4946-8DEF-79B5A660DEFB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532F73EE-1A4C-405F-9BF7-E4C289D84250}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2878,7 +3789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA567FF7-0DE0-44D2-85A7-E9A6F703CCCA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2890,7 +3801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD059EB8-E5D8-4F77-AB24-42EE022CE8ED}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
more on the alien side
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1E2578-D777-46CC-9A39-331AFB17DEED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72F3E42-9BFE-4D23-8A9E-16424F7B3EDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="349">
   <si>
     <t>Name</t>
   </si>
@@ -736,9 +736,6 @@
     <t>Reapers</t>
   </si>
   <si>
-    <t>Biofuel</t>
-  </si>
-  <si>
     <t>Terraforming Earth</t>
   </si>
   <si>
@@ -790,111 +787,9 @@
     <t>d6</t>
   </si>
   <si>
-    <t>Red: -1</t>
-  </si>
-  <si>
-    <t>Red: -1, Purple: -1</t>
-  </si>
-  <si>
-    <t>Red: -2, Purple: -1</t>
-  </si>
-  <si>
-    <t>Red: -2, Purple: -2</t>
-  </si>
-  <si>
     <t>Attack Name</t>
   </si>
   <si>
-    <t>Purple: -1</t>
-  </si>
-  <si>
-    <t>Purple: -2, Green: -1</t>
-  </si>
-  <si>
-    <t>Purple: -3, Green: -2</t>
-  </si>
-  <si>
-    <t>Purple: -3, Green: -3</t>
-  </si>
-  <si>
-    <t>Green: -1</t>
-  </si>
-  <si>
-    <t>Black: -1</t>
-  </si>
-  <si>
-    <t>Yellow: -1</t>
-  </si>
-  <si>
-    <t>Blue: -1</t>
-  </si>
-  <si>
-    <t>Purple: -1, Blue: -1</t>
-  </si>
-  <si>
-    <t>Purple: -1, Blue: -2</t>
-  </si>
-  <si>
-    <t>Purple: -1, , Blue: -2</t>
-  </si>
-  <si>
-    <t>Red: -1, Blue: -2</t>
-  </si>
-  <si>
-    <t>Green: -1, Blue: -1</t>
-  </si>
-  <si>
-    <t>Green: -2, , Blue: -1</t>
-  </si>
-  <si>
-    <t>Green: -1, , Blue: -2</t>
-  </si>
-  <si>
-    <t>Black: -1, Blue: -2</t>
-  </si>
-  <si>
-    <t>Black: -2, Blue: -1</t>
-  </si>
-  <si>
-    <t>Black: -2, Blue: -2</t>
-  </si>
-  <si>
-    <t>Purple: -1, Yellow: -1</t>
-  </si>
-  <si>
-    <t>Purple: -2, , Yellow: -1</t>
-  </si>
-  <si>
-    <t>Purple: -2, Yellow: -3</t>
-  </si>
-  <si>
-    <t>Red: -1, Yellow: -1</t>
-  </si>
-  <si>
-    <t>Green: -1, Yellow: -2</t>
-  </si>
-  <si>
-    <t>Green: -1, Yellow: -3</t>
-  </si>
-  <si>
-    <t>Black: -1, Yellow: -1</t>
-  </si>
-  <si>
-    <t>Blue: -1, Yellow: -1</t>
-  </si>
-  <si>
-    <t>Purple: -1, Black: -1</t>
-  </si>
-  <si>
-    <t>Red: -1, Black: -1</t>
-  </si>
-  <si>
-    <t>Red: -1, Black: -2</t>
-  </si>
-  <si>
-    <t>Red: -2, Black: -2</t>
-  </si>
-  <si>
     <t>Puzzling Miracles</t>
   </si>
   <si>
@@ -914,6 +809,267 @@
   </si>
   <si>
     <t>Zombie Analysts</t>
+  </si>
+  <si>
+    <t>Steel: -1, Insights: -1</t>
+  </si>
+  <si>
+    <t>Steel: -1, Insights: -2</t>
+  </si>
+  <si>
+    <t>Steel: -2, Insights: -2</t>
+  </si>
+  <si>
+    <t>Steel: -3, Insights: -3</t>
+  </si>
+  <si>
+    <t>Insights: -1, Goods: -1</t>
+  </si>
+  <si>
+    <t>Insights: -1, Goods: -2</t>
+  </si>
+  <si>
+    <t>Insights: -1, Goods: -3</t>
+  </si>
+  <si>
+    <t>Insights: -1, Goods: -4</t>
+  </si>
+  <si>
+    <t>Insights: -2</t>
+  </si>
+  <si>
+    <t>Insights: -2, Fear: +1</t>
+  </si>
+  <si>
+    <t>Insights: -2, Fear: +2</t>
+  </si>
+  <si>
+    <t>Insights: -2, Fear: +3</t>
+  </si>
+  <si>
+    <t>Insights: -2, Fear: +4</t>
+  </si>
+  <si>
+    <t>Fear: +1, Food: -1</t>
+  </si>
+  <si>
+    <t>Fear: +1, Food: -2</t>
+  </si>
+  <si>
+    <t>Fear: +1, Food: -3</t>
+  </si>
+  <si>
+    <t>Insights: -3</t>
+  </si>
+  <si>
+    <t>Insights: -4</t>
+  </si>
+  <si>
+    <t>Food: +1, Insights: -2</t>
+  </si>
+  <si>
+    <t>Food: +1, Insights: -1</t>
+  </si>
+  <si>
+    <t>Food: +1, Insights: -3</t>
+  </si>
+  <si>
+    <t>Mysterious Trainwrecks</t>
+  </si>
+  <si>
+    <t>Steel: -2</t>
+  </si>
+  <si>
+    <t>Steel: -3</t>
+  </si>
+  <si>
+    <t>Steel: -4</t>
+  </si>
+  <si>
+    <t>Steel: -5</t>
+  </si>
+  <si>
+    <t>Steel: -1, Servers: -1</t>
+  </si>
+  <si>
+    <t>Steel: -1, Servers: -2</t>
+  </si>
+  <si>
+    <t>Steel: -2, Servers: -2</t>
+  </si>
+  <si>
+    <t>Steel: -2, Servers: -3</t>
+  </si>
+  <si>
+    <t>Steel: -1, Goods: -1</t>
+  </si>
+  <si>
+    <t>Steel: -1, Goods: -2</t>
+  </si>
+  <si>
+    <t>Steel: -1, Goods: -3</t>
+  </si>
+  <si>
+    <t>Steel: -1, Goods: -4</t>
+  </si>
+  <si>
+    <t>Workers: -1</t>
+  </si>
+  <si>
+    <t>Workers: -2</t>
+  </si>
+  <si>
+    <t>Workers: -3</t>
+  </si>
+  <si>
+    <t>Workers: -4</t>
+  </si>
+  <si>
+    <t>Food: -1, Fear: +1</t>
+  </si>
+  <si>
+    <t>Food: -2, Fear: +1</t>
+  </si>
+  <si>
+    <t>Food: -2, Fear: +2</t>
+  </si>
+  <si>
+    <t>Food: -2, Fear: +3</t>
+  </si>
+  <si>
+    <t>Steel: -2, Insight: -1</t>
+  </si>
+  <si>
+    <t>Steel: -2, Insight: -3</t>
+  </si>
+  <si>
+    <t>Steel: -2, Insight: -2</t>
+  </si>
+  <si>
+    <t>Steel: -2, Insight: -4</t>
+  </si>
+  <si>
+    <t>Goods: -1</t>
+  </si>
+  <si>
+    <t>Goods: -2</t>
+  </si>
+  <si>
+    <t>Goods: -3</t>
+  </si>
+  <si>
+    <t>Goods: -4</t>
+  </si>
+  <si>
+    <t>Workers: -3, Food: +1</t>
+  </si>
+  <si>
+    <t>Workers: -4, Food: +2</t>
+  </si>
+  <si>
+    <t>Servers: -1, Food: -1</t>
+  </si>
+  <si>
+    <t>Servers: -1, Food: -2</t>
+  </si>
+  <si>
+    <t>Servers: -2, Food: -2</t>
+  </si>
+  <si>
+    <t>Servers: -3, Food: -3</t>
+  </si>
+  <si>
+    <t>Food: -1, Insights: +1</t>
+  </si>
+  <si>
+    <t>Food: -3, Insights: -2</t>
+  </si>
+  <si>
+    <t>Food: -2, Insights: -1</t>
+  </si>
+  <si>
+    <t>Food: -1</t>
+  </si>
+  <si>
+    <t>Insights: +1, Fear: +1</t>
+  </si>
+  <si>
+    <t>Insights: -4, Fear: +4</t>
+  </si>
+  <si>
+    <t>Steel: +1, Insights: -2</t>
+  </si>
+  <si>
+    <t>Steel: +2, Insights: -3</t>
+  </si>
+  <si>
+    <t>Insights: +1, Fear: +1, Steel: +1</t>
+  </si>
+  <si>
+    <t>Fear: +2, Steel: +2</t>
+  </si>
+  <si>
+    <t>Fear: +3, Steel: +4</t>
+  </si>
+  <si>
+    <t>Fear: +2, Steel: +3</t>
+  </si>
+  <si>
+    <t>Food: -3</t>
+  </si>
+  <si>
+    <t>Food: -4</t>
+  </si>
+  <si>
+    <t>Food: -5</t>
+  </si>
+  <si>
+    <t>EMP Bursts</t>
+  </si>
+  <si>
+    <t>Market Disturbances</t>
+  </si>
+  <si>
+    <t>Disappearing People</t>
+  </si>
+  <si>
+    <t>Novel Illness</t>
+  </si>
+  <si>
+    <t>Radiation Spikes</t>
+  </si>
+  <si>
+    <t>Consumer Shortages</t>
+  </si>
+  <si>
+    <t>Rural Ghost Towns</t>
+  </si>
+  <si>
+    <t>Popular Biohacking</t>
+  </si>
+  <si>
+    <t>The Monoliths</t>
+  </si>
+  <si>
+    <t>Steel: -1, Insights: +1</t>
+  </si>
+  <si>
+    <t>Steel: -2, Insights: +2</t>
+  </si>
+  <si>
+    <t>Chaotic Machinery</t>
+  </si>
+  <si>
+    <t>Energy Breakthroughs</t>
+  </si>
+  <si>
+    <t>Human Biofuel</t>
+  </si>
+  <si>
+    <t>Eco Terrorism</t>
+  </si>
+  <si>
+    <t>Failed Crops</t>
   </si>
 </sst>
 </file>
@@ -3175,7 +3331,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3183,38 +3339,37 @@
     <col min="2" max="2" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="18.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>259</v>
-      </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>253</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -3228,19 +3383,19 @@
         <v>220</v>
       </c>
       <c r="E2" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="G2" t="s">
-        <v>256</v>
-      </c>
-      <c r="H2" t="s">
-        <v>257</v>
-      </c>
-      <c r="I2" t="s">
-        <v>258</v>
+        <v>262</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3254,19 +3409,19 @@
         <v>221</v>
       </c>
       <c r="E3" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="G3" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="I3" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3280,19 +3435,19 @@
         <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -3306,19 +3461,19 @@
         <v>223</v>
       </c>
       <c r="E5" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="F5" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="G5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3332,19 +3487,19 @@
         <v>224</v>
       </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="F6" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="G6" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H6" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3352,25 +3507,25 @@
         <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C7" t="s">
         <v>225</v>
       </c>
       <c r="E7" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="F7" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="G7" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="H7" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="I7" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3383,17 +3538,20 @@
       <c r="C8" t="s">
         <v>226</v>
       </c>
+      <c r="E8" t="s">
+        <v>283</v>
+      </c>
       <c r="F8" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="G8" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
       <c r="H8" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="I8" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3406,17 +3564,20 @@
       <c r="C9" t="s">
         <v>227</v>
       </c>
+      <c r="E9" t="s">
+        <v>333</v>
+      </c>
       <c r="F9" t="s">
-        <v>255</v>
+        <v>288</v>
       </c>
       <c r="G9" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I9" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3429,17 +3590,20 @@
       <c r="C10" t="s">
         <v>228</v>
       </c>
+      <c r="E10" t="s">
+        <v>334</v>
+      </c>
       <c r="F10" t="s">
-        <v>255</v>
+        <v>292</v>
       </c>
       <c r="G10" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="H10" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="I10" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3452,17 +3616,20 @@
       <c r="C11" t="s">
         <v>229</v>
       </c>
+      <c r="E11" t="s">
+        <v>335</v>
+      </c>
       <c r="F11" t="s">
-        <v>255</v>
+        <v>296</v>
       </c>
       <c r="G11" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="H11" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="I11" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -3470,22 +3637,25 @@
         <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C12" t="s">
         <v>230</v>
       </c>
+      <c r="E12" t="s">
+        <v>336</v>
+      </c>
       <c r="F12" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="G12" t="s">
-        <v>255</v>
+        <v>301</v>
       </c>
       <c r="H12" t="s">
-        <v>255</v>
+        <v>302</v>
       </c>
       <c r="I12" t="s">
-        <v>255</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -3498,17 +3668,20 @@
       <c r="C13" t="s">
         <v>231</v>
       </c>
+      <c r="E13" t="s">
+        <v>337</v>
+      </c>
       <c r="F13" t="s">
-        <v>264</v>
+        <v>304</v>
       </c>
       <c r="G13" t="s">
-        <v>264</v>
+        <v>306</v>
       </c>
       <c r="H13" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="I13" t="s">
-        <v>264</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -3521,17 +3694,20 @@
       <c r="C14" t="s">
         <v>232</v>
       </c>
+      <c r="E14" t="s">
+        <v>338</v>
+      </c>
       <c r="F14" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="G14" t="s">
-        <v>272</v>
+        <v>309</v>
       </c>
       <c r="H14" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="I14" t="s">
-        <v>274</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3544,17 +3720,20 @@
       <c r="C15" t="s">
         <v>233</v>
       </c>
+      <c r="E15" t="s">
+        <v>339</v>
+      </c>
       <c r="F15" t="s">
-        <v>264</v>
+        <v>296</v>
       </c>
       <c r="G15" t="s">
-        <v>282</v>
+        <v>312</v>
       </c>
       <c r="H15" t="s">
-        <v>283</v>
+        <v>313</v>
       </c>
       <c r="I15" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -3562,22 +3741,25 @@
         <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C16" t="s">
         <v>234</v>
       </c>
+      <c r="E16" t="s">
+        <v>340</v>
+      </c>
       <c r="F16" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="G16" t="s">
-        <v>264</v>
+        <v>315</v>
       </c>
       <c r="H16" t="s">
-        <v>264</v>
+        <v>316</v>
       </c>
       <c r="I16" t="s">
-        <v>264</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -3590,17 +3772,20 @@
       <c r="C17" t="s">
         <v>235</v>
       </c>
+      <c r="E17" t="s">
+        <v>341</v>
+      </c>
       <c r="F17" t="s">
+        <v>342</v>
+      </c>
+      <c r="G17" t="s">
+        <v>343</v>
+      </c>
+      <c r="H17" t="s">
+        <v>285</v>
+      </c>
+      <c r="I17" t="s">
         <v>265</v>
-      </c>
-      <c r="G17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H17" t="s">
-        <v>276</v>
-      </c>
-      <c r="I17" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -3613,17 +3798,20 @@
       <c r="C18" t="s">
         <v>236</v>
       </c>
+      <c r="E18" t="s">
+        <v>344</v>
+      </c>
       <c r="F18" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="G18" t="s">
-        <v>284</v>
+        <v>321</v>
       </c>
       <c r="H18" t="s">
-        <v>284</v>
+        <v>320</v>
       </c>
       <c r="I18" t="s">
-        <v>284</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3631,22 +3819,25 @@
         <v>215</v>
       </c>
       <c r="B19" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>346</v>
+      </c>
+      <c r="E19" t="s">
+        <v>345</v>
       </c>
       <c r="F19" t="s">
-        <v>265</v>
+        <v>322</v>
       </c>
       <c r="G19" t="s">
-        <v>265</v>
+        <v>322</v>
       </c>
       <c r="H19" t="s">
-        <v>265</v>
+        <v>322</v>
       </c>
       <c r="I19" t="s">
-        <v>265</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -3657,19 +3848,22 @@
         <v>214</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="E20" t="s">
+        <v>347</v>
       </c>
       <c r="F20" t="s">
-        <v>267</v>
+        <v>324</v>
       </c>
       <c r="G20" t="s">
-        <v>285</v>
+        <v>325</v>
       </c>
       <c r="H20" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="I20" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3677,22 +3871,25 @@
         <v>213</v>
       </c>
       <c r="B21" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C21" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>267</v>
+        <v>326</v>
       </c>
       <c r="G21" t="s">
-        <v>267</v>
+        <v>327</v>
       </c>
       <c r="H21" t="s">
-        <v>267</v>
+        <v>329</v>
       </c>
       <c r="I21" t="s">
-        <v>267</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -3700,22 +3897,25 @@
         <v>214</v>
       </c>
       <c r="B22" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C22" t="s">
         <v>217</v>
       </c>
+      <c r="E22" t="s">
+        <v>348</v>
+      </c>
       <c r="F22" t="s">
-        <v>266</v>
+        <v>321</v>
       </c>
       <c r="G22" t="s">
-        <v>266</v>
+        <v>330</v>
       </c>
       <c r="H22" t="s">
-        <v>266</v>
+        <v>331</v>
       </c>
       <c r="I22" t="s">
-        <v>266</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3743,33 +3943,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
         <v>245</v>
-      </c>
-      <c r="B5" t="s">
-        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing, simulating team traits
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6D559C-49A9-474F-8121-50EA69BA0D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1BE357-FC8A-4881-A29C-B2CE3862DDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opportunities" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="Quests" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Opportunities!$A$1:$T$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Experts!$A$1:$O$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Opportunities!$A$1:$U$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="420">
   <si>
     <t>Name</t>
   </si>
@@ -1042,9 +1043,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Power</t>
-  </si>
-  <si>
     <t>James</t>
   </si>
   <si>
@@ -1093,9 +1091,6 @@
     <t>Mason</t>
   </si>
   <si>
-    <t>Rudy</t>
-  </si>
-  <si>
     <t>Mel</t>
   </si>
   <si>
@@ -1144,15 +1139,9 @@
     <t>Leader</t>
   </si>
   <si>
-    <t>-5 with another Leader</t>
-  </si>
-  <si>
     <t>Tag</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -1168,45 +1157,18 @@
     <t>Tactical</t>
   </si>
   <si>
-    <t>Strategist</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>+10 with Creative, +5 Linguist or Engineer</t>
   </si>
   <si>
-    <t>+4 for each other Creative, +5 for Engineer or Officer</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Strategic</t>
   </si>
   <si>
-    <t>Calc. Power</t>
-  </si>
-  <si>
-    <t>Power Adj</t>
-  </si>
-  <si>
-    <t>+5 with Strategist, +6 for Engineer or Officer</t>
-  </si>
-  <si>
-    <t>+1 for each Tactical, +5 for Officer</t>
-  </si>
-  <si>
     <t>Endgame</t>
   </si>
   <si>
     <t>Develop Vaccine: Gain 20 Results insight, Lower Fear to 10</t>
   </si>
   <si>
-    <t>+3 for each Trait in team, +1 for Theologian</t>
-  </si>
-  <si>
     <t>Ideas</t>
   </si>
   <si>
@@ -1259,6 +1221,72 @@
   </si>
   <si>
     <t>Give you Crystals but expects them in return</t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>-3 with another Leader</t>
+  </si>
+  <si>
+    <t>+5 with Strategic, +6 for Engineer or Officer</t>
+  </si>
+  <si>
+    <t>+3 for each Creative, +5 for Officer</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>+2 for each Trait in team, +1 for Theologian</t>
+  </si>
+  <si>
+    <t>leader</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>creative</t>
+  </si>
+  <si>
+    <t>tactical</t>
+  </si>
+  <si>
+    <t>strategic</t>
+  </si>
+  <si>
+    <t>holistic</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>leaderDesc</t>
+  </si>
+  <si>
+    <t>logicalDesc</t>
+  </si>
+  <si>
+    <t>creativeDesc</t>
+  </si>
+  <si>
+    <t>tacticalDesc</t>
+  </si>
+  <si>
+    <t>strategicDesc</t>
+  </si>
+  <si>
+    <t>holisticDesc</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>+5 for each other Creative, +5 for Linguist or Theologian</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1460,9 +1488,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1830,11 +1855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1842,27 +1867,28 @@
     <col min="1" max="1" width="25.81640625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.54296875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="15.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.26953125" style="14" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="10.08984375" style="11" customWidth="1"/>
-    <col min="19" max="19" width="11.26953125" style="16" customWidth="1"/>
-    <col min="20" max="20" width="10.6328125" style="11" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="11"/>
+    <col min="4" max="4" width="6.81640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.26953125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="11.54296875" style="11" customWidth="1"/>
+    <col min="19" max="19" width="10.08984375" style="11" customWidth="1"/>
+    <col min="20" max="20" width="11.26953125" style="16" customWidth="1"/>
+    <col min="21" max="21" width="10.6328125" style="11" customWidth="1"/>
+    <col min="22" max="16384" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1870,89 +1896,89 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D1" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="27">
+      <c r="E2" s="26">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="9"/>
-      <c r="S2" s="10"/>
-    </row>
-    <row r="3" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="9"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="L2" s="30"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="9"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>183</v>
       </c>
@@ -1960,71 +1986,73 @@
         <v>8</v>
       </c>
       <c r="C3" s="11"/>
-      <c r="D3" s="28">
+      <c r="D3" s="11"/>
+      <c r="E3" s="27">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="11" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="32">
+      <c r="L3" s="31">
         <v>2</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="11" t="s">
+      <c r="N3" s="12"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="11"/>
-    </row>
-    <row r="4" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S3" s="11"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="11"/>
-      <c r="D4" s="28">
+      <c r="D4" s="11"/>
+      <c r="E4" s="27">
         <v>3</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="11" t="s">
-        <v>398</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="L4" s="31"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="11"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="14"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="11"/>
-    </row>
-    <row r="5" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S4" s="11"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="11"/>
+    </row>
+    <row r="5" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>160</v>
       </c>
@@ -2032,37 +2060,38 @@
         <v>8</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="28">
+      <c r="D5" s="11"/>
+      <c r="E5" s="27">
         <v>3</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="11" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="K5" s="32">
+      <c r="L5" s="31">
         <v>4</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="11" t="s">
+      <c r="N5" s="12"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="R5" s="11"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="11"/>
-    </row>
-    <row r="6" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S5" s="11"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -2070,41 +2099,42 @@
         <v>8</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="28">
+      <c r="D6" s="11"/>
+      <c r="E6" s="27">
         <v>2</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="32">
+      <c r="L6" s="31">
         <v>4</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M6" s="12"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="11" t="s">
+      <c r="N6" s="12"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="11"/>
-    </row>
-    <row r="7" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S6" s="11"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="11"/>
+    </row>
+    <row r="7" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>45</v>
       </c>
@@ -2112,1156 +2142,1159 @@
         <v>8</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="28">
+      <c r="D7" s="11"/>
+      <c r="E7" s="27">
         <v>2</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="11" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="K7" s="32">
+      <c r="L7" s="31">
         <v>3</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M7" s="12"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="11" t="s">
+      <c r="N7" s="12"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="R7" s="11"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="11"/>
-    </row>
-    <row r="8" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S7" s="11"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="11"/>
+    </row>
+    <row r="8" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="28" t="s">
-        <v>405</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="11"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="L8" s="31"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="14"/>
       <c r="R8" s="11"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S8" s="11"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="11"/>
+    </row>
+    <row r="9" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="28" t="s">
-        <v>401</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="32" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>402</v>
-      </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="R9" s="11"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="M9" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="N9" s="12"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="S9" s="11"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="11"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>132</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="28" t="str">
+      <c r="E10" s="27" t="str">
         <f>"1:1"</f>
         <v>1:1</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>136</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="28" t="str">
+      <c r="E11" s="27" t="str">
         <f>"1:X"</f>
         <v>1:X</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="Q11" s="11" t="s">
+      <c r="R11" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="28" t="str">
+      <c r="E12" s="27" t="str">
         <f>"8:1"</f>
         <v>8:1</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="H12" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="K12" s="28"/>
-      <c r="Q12" s="11" t="s">
+      <c r="L12" s="27"/>
+      <c r="R12" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>194</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="28">
+      <c r="E13" s="27">
         <v>1</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="I13" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>191</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="28" t="str">
+      <c r="E14" s="27" t="str">
         <f>"3:1"</f>
         <v>3:1</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="F14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="Q14" s="11" t="str">
+      <c r="R14" s="11" t="str">
         <f>"-1 Secrecy"</f>
         <v>-1 Secrecy</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>150</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="28" t="str">
+      <c r="E15" s="27" t="str">
         <f>"3:1"</f>
         <v>3:1</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="12">
+      <c r="I15" s="12">
         <v>2</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="O15" s="12">
+      <c r="P15" s="12">
         <v>1</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="Q15" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="Q15" s="11" t="s">
+      <c r="R15" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="G16" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="H16" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="L16" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="M16" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="N16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="N16" s="13" t="s">
+      <c r="O16" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="G17" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="H17" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="12">
+      <c r="I17" s="12">
         <v>2</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K17" s="33" t="s">
+      <c r="L17" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="M17" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="N17" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="N17" s="13" t="s">
+      <c r="O17" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="E18" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="H18" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="33" t="s">
+      <c r="L18" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="M18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N18" s="13" t="s">
+      <c r="O18" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="28">
+      <c r="E19" s="27">
         <v>5</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="J19" s="11" t="s">
+      <c r="H19" s="18"/>
+      <c r="K19" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="28">
+      <c r="E20" s="27">
         <v>2</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>138</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="28" t="str">
+      <c r="E21" s="27" t="str">
         <f>"5:6"</f>
         <v>5:6</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="H21" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="K21" s="32" t="str">
+      <c r="L21" s="31" t="str">
         <f>"3:4"</f>
         <v>3:4</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="N21" s="13" t="s">
+      <c r="O21" s="13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="28">
+      <c r="E22" s="27">
         <v>2</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="J22" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="28">
+      <c r="E23" s="27">
         <v>1</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="13"/>
+      <c r="I23" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J23" s="11" t="s">
+      <c r="K23" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="28">
+      <c r="E24" s="27">
         <v>2</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="N24" s="13" t="s">
+      <c r="O24" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="28">
+      <c r="E25" s="27">
         <v>3</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="F25" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="11" t="s">
+      <c r="H25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="N25" s="13" t="s">
+      <c r="O25" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="E26" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="G26" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="H26" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="E27" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="H27" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="33" t="s">
+      <c r="L27" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="L27" s="13" t="s">
+      <c r="M27" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="N27" s="13" t="s">
+      <c r="O27" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="E28" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="H28" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="K28" s="33" t="s">
+      <c r="L28" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="M28" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="O28" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="28">
+      <c r="E29" s="27">
         <v>1</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="18"/>
+      <c r="I29" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="J29" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="K29" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K29" s="32">
+      <c r="L29" s="31">
         <v>2</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="M29" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Q29" s="11" t="s">
+      <c r="R29" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D30" s="28">
+      <c r="E30" s="27">
         <v>1</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J30" s="11" t="s">
+      <c r="K30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="N30" s="13" t="s">
+      <c r="O30" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="O30" s="12">
+      <c r="P30" s="12">
         <v>1</v>
       </c>
-      <c r="P30" s="14" t="s">
+      <c r="Q30" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="E31" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="H31" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="K31" s="32">
+      <c r="L31" s="31">
         <v>1</v>
       </c>
-      <c r="L31" s="13" t="s">
+      <c r="M31" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="R31" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>193</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D32" s="28" t="str">
+      <c r="E32" s="27" t="str">
         <f>"2:1"</f>
         <v>2:1</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="H32" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="Q32" s="11" t="str">
+      <c r="R32" s="11" t="str">
         <f>"-1 Secrecy for each Military Problem discovered"</f>
         <v>-1 Secrecy for each Military Problem discovered</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>189</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="28" t="str">
+      <c r="E33" s="27" t="str">
         <f>"5:1"</f>
         <v>5:1</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="H33" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="I33" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="J33" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O33" s="12" t="s">
+      <c r="P33" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="P33" s="14" t="s">
+      <c r="Q33" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>146</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D34" s="28" t="str">
+      <c r="E34" s="27" t="str">
         <f>"3:1"</f>
         <v>3:1</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="F34" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="H34" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="H34" s="12">
+      <c r="I34" s="12">
         <v>2</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="J34" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O34" s="12">
+      <c r="P34" s="12">
         <v>1</v>
       </c>
-      <c r="P34" s="14" t="s">
+      <c r="Q34" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="Q34" s="11" t="s">
+      <c r="R34" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="29" t="str">
+      <c r="E35" s="28" t="str">
         <f>"1:2"</f>
         <v>1:2</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="F35" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="G35" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="H35" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="K35" s="33" t="s">
+      <c r="L35" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="M35" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M35" s="12" t="s">
+      <c r="N35" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="N35" s="13" t="s">
+      <c r="O35" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>179</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="E36" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="F36" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="H36" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="E37" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="H37" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="12">
+      <c r="I37" s="12">
         <v>1</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="J37" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K37" s="33" t="s">
+      <c r="L37" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="L37" s="13" t="s">
+      <c r="M37" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="N37" s="13" t="s">
+      <c r="O37" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>178</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="28" t="str">
+      <c r="E38" s="27" t="str">
         <f>"6:3"</f>
         <v>6:3</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="F38" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="H38" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="H38" s="12">
+      <c r="I38" s="12">
         <v>2</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="J38" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="E39" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="F39" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="H39" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="K39" s="33" t="s">
+      <c r="L39" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="L39" s="13" t="s">
+      <c r="M39" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N39" s="13" t="s">
+      <c r="O39" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="E40" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="F40" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="H40" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="K40" s="33" t="s">
+      <c r="L40" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="L40" s="13" t="s">
+      <c r="M40" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N40" s="13" t="s">
+      <c r="O40" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>153</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D41" s="28">
+      <c r="E41" s="27">
         <v>3</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="F41" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="H41" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="H41" s="12">
+      <c r="I41" s="12">
         <v>2</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="J41" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="O41" s="12">
+      <c r="P41" s="12">
         <v>1</v>
       </c>
-      <c r="P41" s="14" t="s">
+      <c r="Q41" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="Q41" s="11" t="s">
+      <c r="R41" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="G42" s="13"/>
-      <c r="S42" s="16" t="s">
+      <c r="H42" s="13"/>
+      <c r="T42" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="T42" s="11" t="s">
+      <c r="U42" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>155</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="28">
+      <c r="E43" s="27">
         <v>1</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="F43" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G43" s="13"/>
-      <c r="J43" s="11" t="s">
+      <c r="H43" s="13"/>
+      <c r="K43" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="S43" s="16" t="s">
+      <c r="T43" s="16" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>170</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G44" s="18"/>
-      <c r="S44" s="16" t="s">
+      <c r="H44" s="18"/>
+      <c r="T44" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="T44" s="11" t="s">
+      <c r="U44" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="28">
+      <c r="E45" s="27">
         <v>1</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="F45" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G45" s="18"/>
-      <c r="J45" s="11" t="s">
+      <c r="H45" s="18"/>
+      <c r="K45" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="S45" s="16" t="s">
+      <c r="T45" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H46" s="12">
+      <c r="I46" s="12">
         <v>1</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="J46" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="S46" s="16" t="s">
+      <c r="T46" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="T46" s="19" t="s">
+      <c r="U46" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G47" s="13"/>
-      <c r="H47" s="12">
+      <c r="H47" s="13"/>
+      <c r="I47" s="12">
         <v>2</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="J47" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="S47" s="16" t="s">
+      <c r="T47" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="T47" s="11" t="s">
+      <c r="U47" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I48" s="13" t="s">
+      <c r="J48" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="P48" s="14" t="s">
+      <c r="Q48" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="S48" s="16" t="s">
+      <c r="T48" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="T48" s="11" t="s">
+      <c r="U48" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>165</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="18"/>
-      <c r="I49" s="13" t="s">
+      <c r="H49" s="18"/>
+      <c r="J49" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="S49" s="16" t="s">
+      <c r="T49" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="T49" s="11" t="s">
+      <c r="U49" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="S50" s="16" t="s">
+      <c r="T50" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="T50" s="11" t="s">
+      <c r="U50" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>172</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="H51" s="12">
+      <c r="I51" s="12">
         <v>1</v>
       </c>
-      <c r="I51" s="13" t="s">
+      <c r="J51" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="T51" s="11" t="s">
+      <c r="U51" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="S52" s="16" t="s">
+      <c r="T52" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="T52" s="11" t="s">
+      <c r="U52" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="G53" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="H53" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H53" s="12">
+      <c r="I53" s="12">
         <v>2</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="J53" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="M53" s="12" t="s">
+      <c r="N53" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="N53" s="13" t="s">
+      <c r="O53" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="O53" s="12">
+      <c r="P53" s="12">
         <v>1</v>
       </c>
-      <c r="P53" s="14" t="s">
+      <c r="Q53" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
         <v>121</v>
       </c>
@@ -3269,18 +3302,19 @@
         <v>120</v>
       </c>
       <c r="C54" s="17"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18" t="s">
+      <c r="D54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="17" t="s">
+      <c r="Q54" s="18"/>
+      <c r="R54" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="R54" s="17"/>
-      <c r="T54" s="17"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S54" s="17"/>
+      <c r="U54" s="17"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>126</v>
       </c>
@@ -3288,18 +3322,19 @@
         <v>120</v>
       </c>
       <c r="C55" s="17"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18" t="s">
+      <c r="D55" s="17"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="17" t="s">
+      <c r="Q55" s="18"/>
+      <c r="R55" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="R55" s="17"/>
-      <c r="T55" s="17"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S55" s="17"/>
+      <c r="U55" s="17"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>122</v>
       </c>
@@ -3307,18 +3342,19 @@
         <v>120</v>
       </c>
       <c r="C56" s="17"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18" t="s">
+      <c r="D56" s="17"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="17" t="s">
+      <c r="Q56" s="18"/>
+      <c r="R56" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="R56" s="17"/>
-      <c r="T56" s="17"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S56" s="17"/>
+      <c r="U56" s="17"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>128</v>
       </c>
@@ -3326,18 +3362,19 @@
         <v>120</v>
       </c>
       <c r="C57" s="17"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18" t="s">
+      <c r="D57" s="17"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="17" t="s">
+      <c r="Q57" s="18"/>
+      <c r="R57" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="R57" s="17"/>
-      <c r="T57" s="17"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S57" s="17"/>
+      <c r="U57" s="17"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>130</v>
       </c>
@@ -3345,82 +3382,83 @@
         <v>120</v>
       </c>
       <c r="C58" s="17"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18" t="s">
+      <c r="D58" s="17"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="P58" s="18"/>
-      <c r="Q58" s="17" t="s">
+      <c r="Q58" s="18"/>
+      <c r="R58" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="R58" s="17"/>
-      <c r="T58" s="17"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S58" s="17"/>
+      <c r="U58" s="17"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D59" s="29"/>
-      <c r="F59" s="14" t="s">
+      <c r="E59" s="28"/>
+      <c r="G59" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="H59" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K59" s="33"/>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="L59" s="32"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="F60" s="14" t="s">
+      <c r="E60" s="28"/>
+      <c r="G60" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="H60" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K60" s="33"/>
-      <c r="M60" s="12" t="s">
+      <c r="L60" s="32"/>
+      <c r="N60" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="N60" s="13" t="s">
+      <c r="O60" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G61" s="18"/>
-      <c r="R61" s="11" t="s">
+      <c r="H61" s="18"/>
+      <c r="S61" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>188</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="S62" s="16" t="s">
+      <c r="T62" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="T62" s="11" t="s">
+      <c r="U62" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>197</v>
       </c>
@@ -3428,27 +3466,27 @@
         <v>198</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
         <v>199</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H64" s="12">
+      <c r="I64" s="12">
         <v>3</v>
       </c>
-      <c r="I64" s="13" t="s">
+      <c r="J64" s="13" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T47" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T47">
+  <autoFilter ref="A1:U47" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U47">
       <sortCondition ref="B2:B47"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T62">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U62">
     <sortCondition ref="B2:B62"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3461,7 +3499,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3476,7 +3514,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>235</v>
@@ -3517,13 +3555,13 @@
       <c r="B4" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="28"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="13"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
-      <c r="K4" s="32"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="13"/>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -3539,984 +3577,1502 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFFC8A-FCB9-4750-8362-637190E70039}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="8.7265625" style="23"/>
-    <col min="6" max="6" width="9.54296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.7265625" style="23"/>
-    <col min="9" max="9" width="19.90625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="23"/>
-    <col min="13" max="13" width="29.90625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="1" width="10.26953125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="19.90625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.36328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="37.08984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>371</v>
+        <v>404</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>376</v>
+        <v>405</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>377</v>
+        <v>406</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>378</v>
+        <v>409</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>374</v>
+        <v>418</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>338</v>
+        <v>414</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>337</v>
+        <v>415</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>339</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>375</v>
+        <v>368</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="H2" s="23">
-        <f t="shared" ref="H2:H33" si="0">COUNTA(B2:F2)</f>
+        <v>20</v>
+      </c>
+      <c r="I2" s="23">
+        <f>COUNTA(B2:G2)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="23" t="str">
+        <f>IF(ISBLANK(B2),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K2" s="23" t="str">
+        <f>IF(ISBLANK(C2),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L2" s="23" t="str">
+        <f>IF(ISBLANK(D2),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M2" s="23" t="str">
+        <f>IF(ISBLANK(E2),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N2" s="23" t="str">
+        <f>IF(ISBLANK(F2),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O2" s="23" t="str">
+        <f>IF(ISBLANK(G2),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H3" s="23">
+        <v>13</v>
+      </c>
+      <c r="I3" s="23">
+        <f>COUNTA(B3:G3)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="23" t="str">
+        <f>IF(ISBLANK(B3),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K3" s="23" t="str">
+        <f>IF(ISBLANK(C3),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L3" s="23" t="str">
+        <f>IF(ISBLANK(D3),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M3" s="23" t="str">
+        <f>IF(ISBLANK(E3),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N3" s="23" t="str">
+        <f>IF(ISBLANK(F3),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O3" s="23" t="str">
+        <f>IF(ISBLANK(G3),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="23">
+        <v>14</v>
+      </c>
+      <c r="I4" s="23">
+        <f>COUNTA(B4:G4)</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="23" t="str">
+        <f>IF(ISBLANK(B4),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K4" s="23" t="str">
+        <f>IF(ISBLANK(C4),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L4" s="23" t="str">
+        <f>IF(ISBLANK(D4),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M4" s="23" t="str">
+        <f>IF(ISBLANK(E4),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N4" s="23" t="str">
+        <f>IF(ISBLANK(F4),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O4" s="23" t="str">
+        <f>IF(ISBLANK(G4),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H5" s="23">
+        <v>7</v>
+      </c>
+      <c r="I5" s="23">
+        <f>COUNTA(B5:G5)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="23" t="str">
+        <f>IF(ISBLANK(B5),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K5" s="23" t="str">
+        <f>IF(ISBLANK(C5),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L5" s="23" t="str">
+        <f>IF(ISBLANK(D5),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
+      </c>
+      <c r="M5" s="23" t="str">
+        <f>IF(ISBLANK(E5),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N5" s="23" t="str">
+        <f>IF(ISBLANK(F5),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O5" s="23" t="str">
+        <f>IF(ISBLANK(G5),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H6" s="23">
+        <v>7</v>
+      </c>
+      <c r="I6" s="23">
+        <f>COUNTA(B6:G6)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="23" t="str">
+        <f>IF(ISBLANK(B6),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K6" s="23" t="str">
+        <f>IF(ISBLANK(C6),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L6" s="23" t="str">
+        <f>IF(ISBLANK(D6),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M6" s="23" t="str">
+        <f>IF(ISBLANK(E6),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N6" s="23" t="str">
+        <f>IF(ISBLANK(F6),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O6" s="23" t="str">
+        <f>IF(ISBLANK(G6),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H7" s="23">
+        <v>4</v>
+      </c>
+      <c r="I7" s="23">
+        <f>COUNTA(B7:G7)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="23" t="str">
+        <f>IF(ISBLANK(B7),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K7" s="23" t="str">
+        <f>IF(ISBLANK(C7),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L7" s="23" t="str">
+        <f>IF(ISBLANK(D7),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M7" s="23" t="str">
+        <f>IF(ISBLANK(E7),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N7" s="23" t="str">
+        <f>IF(ISBLANK(F7),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O7" s="23" t="str">
+        <f>IF(ISBLANK(G7),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H8" s="23">
+        <v>12</v>
+      </c>
+      <c r="I8" s="23">
+        <f>COUNTA(B8:G8)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="23" t="str">
+        <f>IF(ISBLANK(B8),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K8" s="23" t="str">
+        <f>IF(ISBLANK(C8),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L8" s="23" t="str">
+        <f>IF(ISBLANK(D8),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M8" s="23" t="str">
+        <f>IF(ISBLANK(E8),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N8" s="23" t="str">
+        <f>IF(ISBLANK(F8),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O8" s="23" t="str">
+        <f>IF(ISBLANK(G8),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H9" s="23">
+        <v>7</v>
+      </c>
+      <c r="I9" s="23">
+        <f>COUNTA(B9:G9)</f>
+        <v>2</v>
+      </c>
+      <c r="J9" s="23" t="str">
+        <f>IF(ISBLANK(B9),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K9" s="23" t="str">
+        <f>IF(ISBLANK(C9),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L9" s="23" t="str">
+        <f>IF(ISBLANK(D9),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M9" s="23" t="str">
+        <f>IF(ISBLANK(E9),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N9" s="23" t="str">
+        <f>IF(ISBLANK(F9),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O9" s="23" t="str">
+        <f>IF(ISBLANK(G9),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="23" t="s">
+        <v>361</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H10" s="23">
+        <v>6</v>
+      </c>
+      <c r="I10" s="23">
+        <f>COUNTA(B10:G10)</f>
+        <v>2</v>
+      </c>
+      <c r="J10" s="23" t="str">
+        <f>IF(ISBLANK(B10),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K10" s="23" t="str">
+        <f>IF(ISBLANK(C10),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L10" s="23" t="str">
+        <f>IF(ISBLANK(D10),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M10" s="23" t="str">
+        <f>IF(ISBLANK(E10),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N10" s="23" t="str">
+        <f>IF(ISBLANK(F10),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O10" s="23" t="str">
+        <f>IF(ISBLANK(G10),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H11" s="23">
+        <v>16</v>
+      </c>
+      <c r="I11" s="23">
+        <f>COUNTA(B11:G11)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="23" t="str">
+        <f>IF(ISBLANK(B11),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K11" s="23" t="str">
+        <f>IF(ISBLANK(C11),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L11" s="23" t="str">
+        <f>IF(ISBLANK(D11),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M11" s="23" t="str">
+        <f>IF(ISBLANK(E11),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N11" s="23" t="str">
+        <f>IF(ISBLANK(F11),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O11" s="23" t="str">
+        <f>IF(ISBLANK(G11),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H12" s="23">
+        <v>5</v>
+      </c>
+      <c r="I12" s="23">
+        <f>COUNTA(B12:G12)</f>
+        <v>2</v>
+      </c>
+      <c r="J12" s="23" t="str">
+        <f>IF(ISBLANK(B12),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K12" s="23" t="str">
+        <f>IF(ISBLANK(C12),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L12" s="23" t="str">
+        <f>IF(ISBLANK(D12),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M12" s="23" t="str">
+        <f>IF(ISBLANK(E12),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N12" s="23" t="str">
+        <f>IF(ISBLANK(F12),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O12" s="23" t="str">
+        <f>IF(ISBLANK(G12),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H13" s="23">
+        <v>6</v>
+      </c>
+      <c r="I13" s="23">
+        <f>COUNTA(B13:G13)</f>
+        <v>2</v>
+      </c>
+      <c r="J13" s="23" t="str">
+        <f>IF(ISBLANK(B13),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K13" s="23" t="str">
+        <f>IF(ISBLANK(C13),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L13" s="23" t="str">
+        <f>IF(ISBLANK(D13),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
+      </c>
+      <c r="M13" s="23" t="str">
+        <f>IF(ISBLANK(E13),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N13" s="23" t="str">
+        <f>IF(ISBLANK(F13),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O13" s="23" t="str">
+        <f>IF(ISBLANK(G13),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H14" s="23">
+        <v>4</v>
+      </c>
+      <c r="I14" s="23">
+        <f>COUNTA(B14:G14)</f>
+        <v>2</v>
+      </c>
+      <c r="J14" s="23" t="str">
+        <f>IF(ISBLANK(B14),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K14" s="23" t="str">
+        <f>IF(ISBLANK(C14),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L14" s="23" t="str">
+        <f>IF(ISBLANK(D14),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
+      </c>
+      <c r="M14" s="23" t="str">
+        <f>IF(ISBLANK(E14),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N14" s="23" t="str">
+        <f>IF(ISBLANK(F14),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O14" s="23" t="str">
+        <f>IF(ISBLANK(G14),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H15" s="23">
+        <v>7</v>
+      </c>
+      <c r="I15" s="23">
+        <f>COUNTA(B15:G15)</f>
+        <v>2</v>
+      </c>
+      <c r="J15" s="23" t="str">
+        <f>IF(ISBLANK(B15),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K15" s="23" t="str">
+        <f>IF(ISBLANK(C15),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L15" s="23" t="str">
+        <f>IF(ISBLANK(D15),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M15" s="23" t="str">
+        <f>IF(ISBLANK(E15),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N15" s="23" t="str">
+        <f>IF(ISBLANK(F15),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O15" s="23" t="str">
+        <f>IF(ISBLANK(G15),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="23" t="s">
+        <v>343</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H16" s="23">
+        <v>6</v>
+      </c>
+      <c r="I16" s="23">
+        <f>COUNTA(B16:G16)</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="23" t="str">
+        <f>IF(ISBLANK(B16),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K16" s="23" t="str">
+        <f>IF(ISBLANK(C16),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L16" s="23" t="str">
+        <f>IF(ISBLANK(D16),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M16" s="23" t="str">
+        <f>IF(ISBLANK(E16),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N16" s="23" t="str">
+        <f>IF(ISBLANK(F16),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O16" s="23" t="str">
+        <f>IF(ISBLANK(G16),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H17" s="23">
         <v>3</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24">
-        <f>IF(ISBLANK(B2),0,10)+IF(ISBLANK(C2),0,10)+IF(ISBLANK(D2),0,10)+IF(ISBLANK(E2),0,10)+IF(ISBLANK(F2),0,10)+IF(ISBLANK(G2),0,10)-H2</f>
-        <v>27</v>
-      </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="23">
-        <f>J2+K2</f>
-        <v>27</v>
-      </c>
-      <c r="M2" s="23" t="str">
-        <f>I2&amp;" "&amp;IF(ISBLANK(B2),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="I17" s="23">
+        <f>COUNTA(B17:G17)</f>
+        <v>2</v>
+      </c>
+      <c r="J17" s="23" t="str">
+        <f>IF(ISBLANK(B17),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K17" s="23" t="str">
+        <f>IF(ISBLANK(C17),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L17" s="23" t="str">
+        <f>IF(ISBLANK(D17),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
+      </c>
+      <c r="M17" s="23" t="str">
+        <f>IF(ISBLANK(E17),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N17" s="23" t="str">
+        <f>IF(ISBLANK(F17),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O17" s="23" t="str">
+        <f>IF(ISBLANK(G17),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H3" s="23">
-        <f t="shared" si="0"/>
+      <c r="C18" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H18" s="23">
+        <v>4</v>
+      </c>
+      <c r="I18" s="23">
+        <f>COUNTA(B18:G18)</f>
         <v>2</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24">
-        <f t="shared" ref="J3:J33" si="1">IF(ISBLANK(B3),0,10)+IF(ISBLANK(C3),0,10)+IF(ISBLANK(D3),0,10)+IF(ISBLANK(E3),0,10)+IF(ISBLANK(F3),0,10)+IF(ISBLANK(G3),0,10)-H3</f>
-        <v>28</v>
-      </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="23">
-        <f t="shared" ref="L3:L33" si="2">J3+K3</f>
-        <v>28</v>
-      </c>
-      <c r="M3" s="23" t="str">
-        <f>I3&amp;" "&amp;IF(ISBLANK(B3),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
-        <v>341</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H4" s="23">
-        <f t="shared" si="0"/>
+      <c r="J18" s="23" t="str">
+        <f>IF(ISBLANK(B18),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K18" s="23" t="str">
+        <f>IF(ISBLANK(C18),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L18" s="23" t="str">
+        <f>IF(ISBLANK(D18),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M18" s="23" t="str">
+        <f>IF(ISBLANK(E18),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N18" s="23" t="str">
+        <f>IF(ISBLANK(F18),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O18" s="23" t="str">
+        <f>IF(ISBLANK(G18),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H19" s="23">
+        <v>15</v>
+      </c>
+      <c r="I19" s="23">
+        <f>COUNTA(B19:G19)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="M4" s="23" t="str">
-        <f>I4&amp;" "&amp;IF(ISBLANK(B4),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
-        <v>342</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H5" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="23">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="M5" s="23" t="str">
-        <f>I5&amp;" "&amp;IF(ISBLANK(B5),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
-        <v>343</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H6" s="23">
-        <f t="shared" si="0"/>
+      <c r="J19" s="23" t="str">
+        <f>IF(ISBLANK(B19),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K19" s="23" t="str">
+        <f>IF(ISBLANK(C19),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L19" s="23" t="str">
+        <f>IF(ISBLANK(D19),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M19" s="23" t="str">
+        <f>IF(ISBLANK(E19),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N19" s="23" t="str">
+        <f>IF(ISBLANK(F19),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O19" s="23" t="str">
+        <f>IF(ISBLANK(G19),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H20" s="23">
+        <v>6</v>
+      </c>
+      <c r="I20" s="23">
+        <f>COUNTA(B20:G20)</f>
         <v>2</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="M6" s="23" t="str">
-        <f>I6&amp;" "&amp;IF(ISBLANK(B6),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
-        <v>344</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H7" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J7" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L7" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="M7" s="23" t="str">
-        <f>I7&amp;" "&amp;IF(ISBLANK(B7),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
-        <v>345</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H8" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J8" s="24">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="L8" s="23">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="M8" s="23" t="str">
-        <f>I8&amp;" "&amp;IF(ISBLANK(B8),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
-        <v>346</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H9" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J9" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L9" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="M9" s="23" t="str">
-        <f>I9&amp;" "&amp;IF(ISBLANK(B9),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
-        <v>347</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H10" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J10" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L10" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="M10" s="23" t="str">
-        <f>I10&amp;" "&amp;IF(ISBLANK(B10),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="23" t="s">
-        <v>348</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H11" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J11" s="24">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="L11" s="23">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="M11" s="23" t="str">
-        <f>I11&amp;" "&amp;IF(ISBLANK(B11),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H12" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J12" s="24">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="L12" s="23">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="M12" s="23" t="str">
-        <f>I12&amp;" "&amp;IF(ISBLANK(B12),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
-        <v>350</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H13" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="24">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="L13" s="23">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="M13" s="23" t="str">
-        <f>I13&amp;" "&amp;IF(ISBLANK(B13),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H14" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J14" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L14" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="M14" s="23" t="str">
-        <f>I14&amp;" "&amp;IF(ISBLANK(B14),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H15" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J15" s="24">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="L15" s="23">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="M15" s="23" t="str">
-        <f>I15&amp;" "&amp;IF(ISBLANK(B15),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
-        <v>353</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H16" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J16" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L16" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="M16" s="23" t="str">
-        <f>I16&amp;" "&amp;IF(ISBLANK(B16),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
-        <v>354</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H17" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J17" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L17" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="M17" s="23" t="str">
-        <f>I17&amp;" "&amp;IF(ISBLANK(B17),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
-        <v>355</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H18" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J18" s="24">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="L18" s="23">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="M18" s="23" t="str">
-        <f>I18&amp;" "&amp;IF(ISBLANK(B18),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
-        <v>356</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H19" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J19" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L19" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="M19" s="23" t="str">
-        <f>I19&amp;" "&amp;IF(ISBLANK(B19),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="23" t="s">
-        <v>357</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H20" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J20" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L20" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
+      <c r="J20" s="23" t="str">
+        <f>IF(ISBLANK(B20),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K20" s="23" t="str">
+        <f>IF(ISBLANK(C20),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L20" s="23" t="str">
+        <f>IF(ISBLANK(D20),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
       </c>
       <c r="M20" s="23" t="str">
-        <f>I20&amp;" "&amp;IF(ISBLANK(B20),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+        <f>IF(ISBLANK(E20),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N20" s="23" t="str">
+        <f>IF(ISBLANK(F20),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O20" s="23" t="str">
+        <f>IF(ISBLANK(G20),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>375</v>
-      </c>
       <c r="D21" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H21" s="23">
-        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="23">
+        <f>COUNTA(B21:G21)</f>
         <v>3</v>
       </c>
-      <c r="J21" s="24">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="L21" s="23">
-        <f t="shared" si="2"/>
-        <v>37</v>
+      <c r="J21" s="23" t="str">
+        <f>IF(ISBLANK(B21),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K21" s="23" t="str">
+        <f>IF(ISBLANK(C21),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L21" s="23" t="str">
+        <f>IF(ISBLANK(D21),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
       </c>
       <c r="M21" s="23" t="str">
-        <f>I21&amp;" "&amp;IF(ISBLANK(B21),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+        <f>IF(ISBLANK(E21),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N21" s="23" t="str">
+        <f>IF(ISBLANK(F21),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O21" s="23" t="str">
+        <f>IF(ISBLANK(G21),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="H22" s="23">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J22" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L22" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
+      <c r="I22" s="23">
+        <f>COUNTA(B22:G22)</f>
+        <v>3</v>
+      </c>
+      <c r="J22" s="23" t="str">
+        <f>IF(ISBLANK(B22),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K22" s="23" t="str">
+        <f>IF(ISBLANK(C22),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L22" s="23" t="str">
+        <f>IF(ISBLANK(D22),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
       </c>
       <c r="M22" s="23" t="str">
-        <f>I22&amp;" "&amp;IF(ISBLANK(B22),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+        <f>IF(ISBLANK(E22),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N22" s="23" t="str">
+        <f>IF(ISBLANK(F22),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O22" s="23" t="str">
+        <f>IF(ISBLANK(G22),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H23" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J23" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L23" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="I23" s="23">
+        <f>COUNTA(B23:G23)</f>
+        <v>3</v>
+      </c>
+      <c r="J23" s="23" t="str">
+        <f>IF(ISBLANK(B23),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K23" s="23" t="str">
+        <f>IF(ISBLANK(C23),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L23" s="23" t="str">
+        <f>IF(ISBLANK(D23),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
       </c>
       <c r="M23" s="23" t="str">
-        <f>I23&amp;" "&amp;IF(ISBLANK(B23),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+        <f>IF(ISBLANK(E23),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N23" s="23" t="str">
+        <f>IF(ISBLANK(F23),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O23" s="23" t="str">
+        <f>IF(ISBLANK(G23),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
-        <v>361</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>375</v>
+        <v>350</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="H24" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J24" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L24" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="I24" s="23">
+        <f>COUNTA(B24:G24)</f>
+        <v>3</v>
+      </c>
+      <c r="J24" s="23" t="str">
+        <f>IF(ISBLANK(B24),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K24" s="23" t="str">
+        <f>IF(ISBLANK(C24),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L24" s="23" t="str">
+        <f>IF(ISBLANK(D24),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
       </c>
       <c r="M24" s="23" t="str">
-        <f>I24&amp;" "&amp;IF(ISBLANK(B24),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+        <f>IF(ISBLANK(E24),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N24" s="23" t="str">
+        <f>IF(ISBLANK(F24),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O24" s="23" t="str">
+        <f>IF(ISBLANK(G24),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
-        <v>362</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>375</v>
+        <v>339</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="H25" s="23">
-        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I25" s="23">
+        <f>COUNTA(B25:G25)</f>
+        <v>3</v>
+      </c>
+      <c r="J25" s="23" t="str">
+        <f>IF(ISBLANK(B25),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K25" s="23" t="str">
+        <f>IF(ISBLANK(C25),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L25" s="23" t="str">
+        <f>IF(ISBLANK(D25),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M25" s="23" t="str">
+        <f>IF(ISBLANK(E25),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N25" s="23" t="str">
+        <f>IF(ISBLANK(F25),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O25" s="23" t="str">
+        <f>IF(ISBLANK(G25),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H26" s="23">
+        <v>5</v>
+      </c>
+      <c r="I26" s="23">
+        <f>COUNTA(B26:G26)</f>
+        <v>3</v>
+      </c>
+      <c r="J26" s="23" t="str">
+        <f>IF(ISBLANK(B26),"",'Expert Tags'!B$2)</f>
+        <v/>
+      </c>
+      <c r="K26" s="23" t="str">
+        <f>IF(ISBLANK(C26),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L26" s="23" t="str">
+        <f>IF(ISBLANK(D26),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M26" s="23" t="str">
+        <f>IF(ISBLANK(E26),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N26" s="23" t="str">
+        <f>IF(ISBLANK(F26),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O26" s="23" t="str">
+        <f>IF(ISBLANK(G26),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H27" s="23">
+        <v>3</v>
+      </c>
+      <c r="I27" s="23">
+        <f>COUNTA(B27:G27)</f>
+        <v>3</v>
+      </c>
+      <c r="J27" s="23" t="str">
+        <f>IF(ISBLANK(B27),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K27" s="23" t="str">
+        <f>IF(ISBLANK(C27),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L27" s="23" t="str">
+        <f>IF(ISBLANK(D27),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M27" s="23" t="str">
+        <f>IF(ISBLANK(E27),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N27" s="23" t="str">
+        <f>IF(ISBLANK(F27),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O27" s="23" t="str">
+        <f>IF(ISBLANK(G27),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H28" s="23">
+        <v>7</v>
+      </c>
+      <c r="I28" s="23">
+        <f>COUNTA(B28:G28)</f>
+        <v>3</v>
+      </c>
+      <c r="J28" s="23" t="str">
+        <f>IF(ISBLANK(B28),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K28" s="23" t="str">
+        <f>IF(ISBLANK(C28),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L28" s="23" t="str">
+        <f>IF(ISBLANK(D28),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
+      </c>
+      <c r="M28" s="23" t="str">
+        <f>IF(ISBLANK(E28),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N28" s="23" t="str">
+        <f>IF(ISBLANK(F28),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O28" s="23" t="str">
+        <f>IF(ISBLANK(G28),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" s="23" t="s">
+        <v>402</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H29" s="23">
+        <v>6</v>
+      </c>
+      <c r="I29" s="23">
+        <f>COUNTA(B29:G29)</f>
+        <v>3</v>
+      </c>
+      <c r="J29" s="23" t="str">
+        <f>IF(ISBLANK(B29),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K29" s="23" t="str">
+        <f>IF(ISBLANK(C29),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L29" s="23" t="str">
+        <f>IF(ISBLANK(D29),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
+      </c>
+      <c r="M29" s="23" t="str">
+        <f>IF(ISBLANK(E29),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N29" s="23" t="str">
+        <f>IF(ISBLANK(F29),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O29" s="23" t="str">
+        <f>IF(ISBLANK(G29),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="23" t="s">
+        <v>338</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H30" s="23">
+        <v>9</v>
+      </c>
+      <c r="I30" s="23">
+        <f>COUNTA(B30:G30)</f>
+        <v>3</v>
+      </c>
+      <c r="J30" s="23" t="str">
+        <f>IF(ISBLANK(B30),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K30" s="23" t="str">
+        <f>IF(ISBLANK(C30),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L30" s="23" t="str">
+        <f>IF(ISBLANK(D30),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M30" s="23" t="str">
+        <f>IF(ISBLANK(E30),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N30" s="23" t="str">
+        <f>IF(ISBLANK(F30),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O30" s="23" t="str">
+        <f>IF(ISBLANK(G30),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="23" t="s">
+        <v>341</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H31" s="23">
+        <v>8</v>
+      </c>
+      <c r="I31" s="23">
+        <f>COUNTA(B31:G31)</f>
+        <v>3</v>
+      </c>
+      <c r="J31" s="23" t="str">
+        <f>IF(ISBLANK(B31),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K31" s="23" t="str">
+        <f>IF(ISBLANK(C31),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L31" s="23" t="str">
+        <f>IF(ISBLANK(D31),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M31" s="23" t="str">
+        <f>IF(ISBLANK(E31),"",'Expert Tags'!B$5)</f>
+        <v>+5 with Strategic, +6 for Engineer or Officer</v>
+      </c>
+      <c r="N31" s="23" t="str">
+        <f>IF(ISBLANK(F31),"",'Expert Tags'!B$6)</f>
+        <v/>
+      </c>
+      <c r="O31" s="23" t="str">
+        <f>IF(ISBLANK(G31),"",'Expert Tags'!B$7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H32" s="23">
         <v>1</v>
       </c>
-      <c r="J25" s="24">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="L25" s="23">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="M25" s="23" t="str">
-        <f>I25&amp;" "&amp;IF(ISBLANK(B25),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="23" t="s">
-        <v>363</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H26" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J26" s="24">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="L26" s="23">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="M26" s="23" t="str">
-        <f>I26&amp;" "&amp;IF(ISBLANK(B26),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
-        <v>364</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H27" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J27" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L27" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="M27" s="23" t="str">
-        <f>I27&amp;" "&amp;IF(ISBLANK(B27),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="23" t="s">
-        <v>365</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H28" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J28" s="24">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="L28" s="23">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="M28" s="23" t="str">
-        <f>I28&amp;" "&amp;IF(ISBLANK(B28),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H29" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J29" s="24">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="L29" s="23">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="M29" s="23" t="str">
-        <f>I29&amp;" "&amp;IF(ISBLANK(B29),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
-        <v>367</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G30" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H30" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J30" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L30" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="M30" s="23" t="str">
-        <f>I30&amp;" "&amp;IF(ISBLANK(B30),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> +3 for each Trait in team, +1 for Theologian</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="23" t="s">
-        <v>368</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="G31" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H31" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J31" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L31" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="M31" s="23" t="str">
-        <f>I31&amp;" "&amp;IF(ISBLANK(B31),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="23" t="s">
-        <v>369</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H32" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J32" s="24">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L32" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
+      <c r="I32" s="23">
+        <f>COUNTA(B32:G32)</f>
+        <v>4</v>
+      </c>
+      <c r="J32" s="23" t="str">
+        <f>IF(ISBLANK(B32),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K32" s="23" t="str">
+        <f>IF(ISBLANK(C32),"",'Expert Tags'!B$3)</f>
+        <v/>
+      </c>
+      <c r="L32" s="23" t="str">
+        <f>IF(ISBLANK(D32),"",'Expert Tags'!B$4)</f>
+        <v>+5 for each other Creative, +5 for Linguist or Theologian</v>
       </c>
       <c r="M32" s="23" t="str">
-        <f>I32&amp;" "&amp;IF(ISBLANK(B32),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+        <f>IF(ISBLANK(E32),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N32" s="23" t="str">
+        <f>IF(ISBLANK(F32),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O32" s="23" t="str">
+        <f>IF(ISBLANK(G32),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
-        <v>370</v>
+        <v>347</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H33" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="24">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L33" s="23">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="I33" s="23">
+        <f>COUNTA(B33:G33)</f>
+        <v>4</v>
+      </c>
+      <c r="J33" s="23" t="str">
+        <f>IF(ISBLANK(B33),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K33" s="23" t="str">
+        <f>IF(ISBLANK(C33),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L33" s="23" t="str">
+        <f>IF(ISBLANK(D33),"",'Expert Tags'!B$4)</f>
+        <v/>
       </c>
       <c r="M33" s="23" t="str">
-        <f>I33&amp;" "&amp;IF(ISBLANK(B33),"",VLOOKUP(B$1, 'Expert Tags'!A:B, 2))</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(E33),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N33" s="23" t="str">
+        <f>IF(ISBLANK(F33),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O33" s="23" t="str">
+        <f>IF(ISBLANK(G33),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A34" s="23" t="s">
+        <v>344</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H34" s="23">
+        <v>5</v>
+      </c>
+      <c r="I34" s="23">
+        <f>COUNTA(B34:G34)</f>
+        <v>4</v>
+      </c>
+      <c r="J34" s="23" t="str">
+        <f>IF(ISBLANK(B34),"",'Expert Tags'!B$2)</f>
+        <v>-3 with another Leader</v>
+      </c>
+      <c r="K34" s="23" t="str">
+        <f>IF(ISBLANK(C34),"",'Expert Tags'!B$3)</f>
+        <v>+10 with Creative, +5 Linguist or Engineer</v>
+      </c>
+      <c r="L34" s="23" t="str">
+        <f>IF(ISBLANK(D34),"",'Expert Tags'!B$4)</f>
+        <v/>
+      </c>
+      <c r="M34" s="23" t="str">
+        <f>IF(ISBLANK(E34),"",'Expert Tags'!B$5)</f>
+        <v/>
+      </c>
+      <c r="N34" s="23" t="str">
+        <f>IF(ISBLANK(F34),"",'Expert Tags'!B$6)</f>
+        <v>+3 for each Creative, +5 for Officer</v>
+      </c>
+      <c r="O34" s="23" t="str">
+        <f>IF(ISBLANK(G34),"",'Expert Tags'!B$7)</f>
+        <v>+2 for each Trait in team, +1 for Theologian</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O34" xr:uid="{FCDFFC8A-FCB9-4750-8362-637190E70039}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O34">
+      <sortCondition ref="I1:I34"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O34">
+    <sortCondition ref="B2:B34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4525,9 +5081,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C158F0A8-90B7-4C4B-8671-E206D9D26AA6}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4537,7 +5093,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>337</v>
@@ -4545,50 +5101,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
+      <c r="B3" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>382</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>378</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
-        <v>379</v>
-      </c>
       <c r="B6" s="21" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
-        <v>380</v>
+      <c r="A7" s="24" t="s">
+        <v>374</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -4642,13 +5198,13 @@
         <v>241</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>234</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -4674,7 +5230,7 @@
         <v>253</v>
       </c>
       <c r="I2" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J2" t="s">
         <v>208</v>
@@ -4703,7 +5259,7 @@
         <v>257</v>
       </c>
       <c r="I3" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="J3" t="s">
         <v>209</v>
@@ -4732,7 +5288,7 @@
         <v>262</v>
       </c>
       <c r="I4" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="J4" t="s">
         <v>210</v>
@@ -4787,7 +5343,7 @@
         <v>267</v>
       </c>
       <c r="I6" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="J6" t="s">
         <v>212</v>
@@ -4842,7 +5398,7 @@
         <v>275</v>
       </c>
       <c r="I8" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="J8" t="s">
         <v>214</v>
@@ -4952,7 +5508,7 @@
         <v>218</v>
       </c>
       <c r="K12" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -4978,7 +5534,7 @@
         <v>295</v>
       </c>
       <c r="I13" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="J13" t="s">
         <v>219</v>

</xml_diff>